<commit_message>
add shift resistor part
</commit_message>
<xml_diff>
--- a/doc/CMD list of Face attendence .xlsx
+++ b/doc/CMD list of Face attendence .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF1FCCC-79AF-409F-8113-A89338B5E21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32C46DE-7B29-433D-B02E-648F0A9AE5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$21:$F$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$22:$F$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="213">
   <si>
     <t>ping</t>
   </si>
@@ -443,140 +443,6 @@
   </si>
   <si>
     <t xml:space="preserve">time&lt;space&gt;24-10-28-1-16-32-05 </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    0   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">          </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">          </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">             </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 4 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">             </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF66FF33"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1001,9 +867,6 @@
     <t>Device Name Read UUID</t>
   </si>
   <si>
-    <t>0x2A01</t>
-  </si>
-  <si>
     <t>0xFF02</t>
   </si>
   <si>
@@ -1371,6 +1234,183 @@
       <t xml:space="preserve">  will be incrimented by 1 for each transection.
 </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Disconnect </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">20 00 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CMD Transection No + 00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0x20 0x00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x05</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0x00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF66FF33"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <t>0x2A00</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1545,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1611,6 +1651,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1736,7 +1782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1804,13 +1850,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1819,9 +1858,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1831,9 +1867,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1843,130 +1876,140 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2315,7 +2358,7 @@
   <dimension ref="A1:N88"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,908 +2380,911 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
-        <v>176</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
+      <c r="A1" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-    </row>
-    <row r="4" spans="1:6" s="47" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91" t="s">
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="63"/>
+    </row>
+    <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="92"/>
-    </row>
-    <row r="5" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="B6" s="46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+    </row>
+    <row r="10" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="65"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="65"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="65"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="90" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="90" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
-      <c r="B8" s="89"/>
-    </row>
-    <row r="9" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-    </row>
-    <row r="10" spans="1:6" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="89"/>
-      <c r="B10" s="89"/>
-    </row>
-    <row r="11" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
-        <v>192</v>
-      </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="81"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="37" t="s">
+      <c r="D17" s="43" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="90"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="D19" s="90"/>
+    </row>
+    <row r="21" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="72" t="s">
         <v>178</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+    </row>
+    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A22" s="82" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="82" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="82" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="36" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="D13" s="83" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="84"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="84"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="84"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
-        <v>208</v>
-      </c>
-      <c r="B17" s="86" t="s">
-        <v>207</v>
-      </c>
-      <c r="C17" s="87" t="s">
-        <v>200</v>
-      </c>
-      <c r="D17" s="88" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="82" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>205</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="D18" s="93"/>
-    </row>
-    <row r="20" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-    </row>
-    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="F21" s="40" t="s">
-        <v>168</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>118</v>
+      <c r="F22" s="82" t="s">
+        <v>167</v>
       </c>
       <c r="G22" s="6"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
+    <row r="23" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="47" t="s">
+        <v>128</v>
+      </c>
       <c r="B23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G23" s="6"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="47"/>
+      <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9" t="s">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="F23" s="12" t="s">
+      <c r="E24" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="68"/>
-      <c r="B24" s="9" t="s">
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="47"/>
+      <c r="B25" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10" t="s">
+      <c r="D25" s="9"/>
+      <c r="E25" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="68"/>
-      <c r="B25" s="10" t="s">
+      <c r="F25" s="12"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="47"/>
+      <c r="B26" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="68"/>
-      <c r="B26" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="47"/>
+      <c r="B27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="9" t="s">
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
+      <c r="B28" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9" t="s">
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
-      <c r="B28" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="68"/>
+    <row r="30" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
       <c r="B30" s="9" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F30" s="9"/>
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="68"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="B33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E33" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F33" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="73"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="75"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="52"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
-      <c r="B35" s="7" t="s">
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
+      <c r="B36" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
-      <c r="B36" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="48"/>
+      <c r="B37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
-      <c r="B37" s="8" t="s">
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="48"/>
+      <c r="B38" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="8" t="s">
+      <c r="C38" s="7"/>
+      <c r="D38" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="73"/>
-      <c r="B38" s="74"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="75"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B40" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="17" t="s">
+      <c r="C40" s="14"/>
+      <c r="D40" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="78"/>
-    </row>
-    <row r="41" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="59" t="s">
+      <c r="E40" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="55"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
+    </row>
+    <row r="42" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B42" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C42" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="23" t="s">
+      <c r="D42" s="22"/>
+      <c r="E42" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
-      <c r="B42" s="22" t="s">
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="75"/>
+      <c r="B43" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22" t="s">
+      <c r="C43" s="22"/>
+      <c r="D43" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E43" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
-      <c r="B43" s="22" t="s">
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="75"/>
+      <c r="B44" s="22" t="s">
         <v>109</v>
-      </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="22" t="s">
-        <v>111</v>
       </c>
       <c r="C44" s="22"/>
       <c r="D44" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="75"/>
+      <c r="B45" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E45" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="22" t="s">
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="75"/>
+      <c r="B46" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C46" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D46" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E46" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
-      <c r="B46" s="22" t="s">
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="75"/>
+      <c r="B47" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="22" t="s">
-        <v>39</v>
       </c>
       <c r="C47" s="22"/>
       <c r="D47" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="59"/>
+      <c r="A48" s="75"/>
       <c r="B48" s="22" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="75"/>
+      <c r="B49" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E49" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F49" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="62"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="64"/>
-    </row>
-    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="78"/>
+      <c r="B50" s="79"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="79"/>
+      <c r="F50" s="80"/>
+    </row>
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="27" t="s">
+      <c r="B51" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="27" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="E50" s="27" t="s">
+      <c r="F51" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F50" s="28" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="49"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="51"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="60" t="s">
+    </row>
+    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="66"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="68"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B53" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C53" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="29"/>
-      <c r="E52" s="30" t="s">
+      <c r="D53" s="29"/>
+      <c r="E53" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F53" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="60"/>
-      <c r="B53" s="29" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="76"/>
+      <c r="B54" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29" t="s">
+      <c r="C54" s="29"/>
+      <c r="D54" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="E54" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F53" s="29"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="60"/>
-      <c r="B54" s="29" t="s">
+      <c r="F54" s="29"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="76"/>
+      <c r="B55" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C55" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30" t="s">
+      <c r="D55" s="29"/>
+      <c r="E55" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F55" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="60"/>
-      <c r="B55" s="29" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="76"/>
+      <c r="B56" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="31" t="s">
+      <c r="C56" s="29"/>
+      <c r="D56" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E56" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F55" s="29"/>
-    </row>
-    <row r="56" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="54"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="61" t="s">
+      <c r="F56" s="29"/>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="69"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="70"/>
+      <c r="F57" s="71"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B58" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C58" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D57" s="13"/>
-      <c r="E57" s="14" t="s">
+      <c r="D58" s="13"/>
+      <c r="E58" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F57" s="13" t="s">
+      <c r="F58" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="61"/>
-      <c r="B58" s="13" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="77"/>
+      <c r="B59" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13" t="s">
+      <c r="C59" s="13"/>
+      <c r="D59" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E59" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F59" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="52"/>
-      <c r="B59" s="53"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="54"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="58" t="s">
+    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="69"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="71"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B61" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C61" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D60" s="15"/>
-      <c r="E60" s="16" t="s">
+      <c r="D61" s="15"/>
+      <c r="E61" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F60" s="15" t="s">
+      <c r="F61" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
-      <c r="B61" s="15" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="74"/>
+      <c r="B62" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15" t="s">
+      <c r="C62" s="15"/>
+      <c r="D62" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E62" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F62" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="41"/>
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="57" t="s">
-        <v>161</v>
-      </c>
-      <c r="B63" s="57"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="57"/>
-      <c r="F63" s="57"/>
-    </row>
-    <row r="65" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="56" t="s">
+    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="37"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" s="58"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="58"/>
+      <c r="F64" s="58"/>
+    </row>
+    <row r="66" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="B66" s="81"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="73" t="s">
+        <v>179</v>
+      </c>
+      <c r="E66" s="73"/>
+    </row>
+    <row r="67" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" s="88" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="B65" s="65"/>
-      <c r="C65" s="65"/>
-      <c r="D65" s="56" t="s">
-        <v>180</v>
-      </c>
-      <c r="E65" s="56"/>
-    </row>
-    <row r="66" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="B66" s="35" t="s">
+    </row>
+    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="D66" s="45" t="s">
+      <c r="D68" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="E66" s="46" t="s">
+      <c r="E68" s="89" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" s="43" t="s">
-        <v>152</v>
-      </c>
-      <c r="D67" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="E67" s="48" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="4">
-        <v>1</v>
-      </c>
-      <c r="C68" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
     </row>
     <row r="69" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="5">
-        <v>45575.507002314815</v>
-      </c>
-      <c r="C69" s="43"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
+        <v>71</v>
+      </c>
+      <c r="B69" s="4">
+        <v>1</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D69" s="89"/>
+      <c r="E69" s="89"/>
     </row>
     <row r="70" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="5">
+        <v>45575.507002314815</v>
+      </c>
+      <c r="C70" s="39"/>
+      <c r="D70" s="89"/>
+      <c r="E70" s="89"/>
+    </row>
+    <row r="71" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-    </row>
-    <row r="71" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="43"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
+      <c r="C71" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71" s="89"/>
+      <c r="E71" s="89"/>
     </row>
     <row r="72" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
@@ -3247,22 +3293,22 @@
       <c r="B72" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="43" t="s">
+      <c r="C72" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
+      <c r="D72" s="89"/>
+      <c r="E72" s="89"/>
     </row>
     <row r="73" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B73" s="4"/>
-      <c r="C73" s="43" t="s">
+      <c r="C73" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
+      <c r="D73" s="89"/>
+      <c r="E73" s="89"/>
     </row>
     <row r="74" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
@@ -3271,11 +3317,11 @@
       <c r="B74" s="4">
         <v>11000</v>
       </c>
-      <c r="C74" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
+      <c r="C74" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D74" s="89"/>
+      <c r="E74" s="89"/>
     </row>
     <row r="75" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
@@ -3284,11 +3330,11 @@
       <c r="B75" s="4">
         <v>100</v>
       </c>
-      <c r="C75" s="43" t="s">
+      <c r="C75" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="D75" s="48"/>
-      <c r="E75" s="48"/>
+      <c r="D75" s="89"/>
+      <c r="E75" s="89"/>
     </row>
     <row r="76" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
@@ -3297,11 +3343,11 @@
       <c r="B76" s="4">
         <v>110</v>
       </c>
-      <c r="C76" s="43" t="s">
+      <c r="C76" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
+      <c r="D76" s="89"/>
+      <c r="E76" s="89"/>
     </row>
     <row r="77" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
@@ -3310,132 +3356,133 @@
       <c r="B77" s="4">
         <v>11</v>
       </c>
-      <c r="C77" s="43" t="s">
+      <c r="C77" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D77" s="48"/>
-      <c r="E77" s="48"/>
+      <c r="D77" s="89"/>
+      <c r="E77" s="89"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="70" t="s">
+      <c r="A78" s="49" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="33" t="s">
+      <c r="B78" s="85" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="86"/>
+      <c r="D78" s="89"/>
+      <c r="E78" s="89"/>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="50"/>
+      <c r="B79" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="C78" s="44"/>
-      <c r="D78" s="48"/>
-      <c r="E78" s="48"/>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="71"/>
-      <c r="B79" s="66" t="s">
-        <v>135</v>
-      </c>
-      <c r="C79" s="67"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
+      <c r="C79" s="84"/>
+      <c r="D79" s="89"/>
+      <c r="E79" s="89"/>
     </row>
     <row r="80" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C80" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
+      <c r="C80" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D80" s="89"/>
+      <c r="E80" s="89"/>
     </row>
     <row r="81" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C81" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
+      <c r="C81" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D81" s="89"/>
+      <c r="E81" s="89"/>
     </row>
     <row r="82" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B82" s="4">
         <v>6</v>
       </c>
-      <c r="C82" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="D82" s="48"/>
-      <c r="E82" s="48"/>
+      <c r="C82" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D82" s="89"/>
+      <c r="E82" s="89"/>
     </row>
     <row r="83" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B83" s="4">
         <v>10</v>
       </c>
-      <c r="C83" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="D83" s="48"/>
-      <c r="E83" s="48"/>
+      <c r="C83" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="89"/>
+      <c r="E83" s="89"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D84" s="42"/>
-      <c r="E84" s="42"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D86" s="42"/>
-      <c r="E86" s="42"/>
+      <c r="D86" s="38"/>
+      <c r="E86" s="38"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D87" s="42"/>
-      <c r="E87" s="42"/>
+      <c r="D87" s="38"/>
+      <c r="E87" s="38"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D88" s="42"/>
-      <c r="E88" s="42"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A22:A32"/>
-    <mergeCell ref="A34:A37"/>
+  <mergeCells count="27">
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="A35:A38"/>
     <mergeCell ref="A78:A79"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A38:F38"/>
-    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A39:F39"/>
+    <mergeCell ref="A41:F41"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D67:D83"/>
-    <mergeCell ref="E67:E83"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A59:F59"/>
-    <mergeCell ref="A20:F20"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D68:D83"/>
+    <mergeCell ref="E68:E83"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A60:F60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
wifi retrying feedback in ble
</commit_message>
<xml_diff>
--- a/doc/CMD list of Face attendence .xlsx
+++ b/doc/CMD list of Face attendence .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32C46DE-7B29-433D-B02E-648F0A9AE5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10598126-CF68-49A6-B2CE-4CC726A9F34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$22:$F$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$23:$F$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="217">
   <si>
     <t>ping</t>
   </si>
@@ -1130,58 +1130,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Transection No</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> indipendent from </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="2"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CMD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="2"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Transection No</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">4D 04 + </t>
     </r>
     <r>
@@ -1411,6 +1359,125 @@
   </si>
   <si>
     <t>0x2A00</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4D 04 + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transection No</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + len +0x74 0x72 0x79</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">0x4D 0x04 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0x00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0x030x74 0x72 0x79</t>
+    </r>
+  </si>
+  <si>
+    <t>Connection trying</t>
+  </si>
+  <si>
+    <t>CMD From Device</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transection No</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> indipendent from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CMD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Transection No.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+it's also incrimented by 1 for each transection.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1661,7 +1728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1778,11 +1845,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1877,140 +1964,160 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2355,10 +2462,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N88"/>
+  <dimension ref="A1:N89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,28 +2487,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="63"/>
+      <c r="B4" s="78"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -2412,10 +2519,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2424,7 +2531,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
@@ -2432,1011 +2539,1031 @@
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="76" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
     </row>
     <row r="10" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="79" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="33" t="s">
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="80"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>177</v>
       </c>
       <c r="C12" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="E12" s="33" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52" t="s">
         <v>169</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="66"/>
+      <c r="D13" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="D13" s="64" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+      <c r="E13" s="63" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52" t="s">
         <v>140</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="68"/>
+      <c r="D14" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="D14" s="65"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="E14" s="64"/>
+    </row>
+    <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52" t="s">
         <v>141</v>
       </c>
       <c r="B15" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="68"/>
+      <c r="D15" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="D15" s="65"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="E15" s="64"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
         <v>142</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="68"/>
+      <c r="D16" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="D16" s="65"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="B17" s="44" t="s">
+      <c r="E16" s="64"/>
+    </row>
+    <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="68"/>
+      <c r="D17" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="64"/>
+    </row>
+    <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
+        <v>207</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="67"/>
+      <c r="D18" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" s="65"/>
+    </row>
+    <row r="19" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="B19" s="66"/>
+      <c r="C19" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="B20" s="67"/>
+      <c r="C20" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="D17" s="43" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="D18" s="90"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>208</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>210</v>
-      </c>
-      <c r="D19" s="90"/>
-    </row>
-    <row r="21" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="72" t="s">
+      <c r="E20" s="62"/>
+    </row>
+    <row r="22" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-    </row>
-    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A22" s="82" t="s">
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+    </row>
+    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A23" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B23" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="82" t="s">
+      <c r="C23" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="82" t="s">
+      <c r="D23" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="82" t="s">
+      <c r="E23" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="F22" s="82" t="s">
+      <c r="F23" s="46" t="s">
         <v>167</v>
-      </c>
-      <c r="G22" s="6"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="G23" s="6"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
+    <row r="24" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="94" t="s">
+        <v>128</v>
+      </c>
       <c r="B24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="94"/>
+      <c r="B25" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F25" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="9" t="s">
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="94"/>
+      <c r="B26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="10" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="94"/>
+      <c r="B27" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="94"/>
+      <c r="B28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="9" t="s">
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="94"/>
+      <c r="B29" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="94"/>
       <c r="B30" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+    <row r="31" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="94"/>
       <c r="B31" s="9" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F31" s="9"/>
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="94"/>
       <c r="B32" s="9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="94"/>
       <c r="B33" s="9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="94"/>
+      <c r="B34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E34" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F34" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="54"/>
       <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="95" t="s">
         <v>127</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D36" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E36" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
-      <c r="B36" s="7" t="s">
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="95"/>
+      <c r="B37" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
-      <c r="B37" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="95"/>
+      <c r="B38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E38" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="48"/>
-      <c r="B38" s="8" t="s">
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="95"/>
+      <c r="B39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8" t="s">
+      <c r="C39" s="7"/>
+      <c r="D39" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="54"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="70"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B41" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="17" t="s">
+      <c r="C41" s="14"/>
+      <c r="D41" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E41" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F40" s="18" t="s">
+      <c r="F41" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57"/>
-    </row>
-    <row r="42" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="75" t="s">
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="73"/>
+      <c r="B42" s="74"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="75"/>
+    </row>
+    <row r="43" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B43" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C43" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="23" t="s">
+      <c r="D43" s="22"/>
+      <c r="E43" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="75"/>
-      <c r="B43" s="22" t="s">
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="87"/>
+      <c r="B44" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22" t="s">
+      <c r="C44" s="22"/>
+      <c r="D44" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E44" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="75"/>
-      <c r="B44" s="22" t="s">
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="87"/>
+      <c r="B45" s="22" t="s">
         <v>109</v>
-      </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="75"/>
-      <c r="B45" s="22" t="s">
-        <v>111</v>
       </c>
       <c r="C45" s="22"/>
       <c r="D45" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="87"/>
+      <c r="B46" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="22"/>
+      <c r="D46" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E46" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="75"/>
-      <c r="B46" s="22" t="s">
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="87"/>
+      <c r="B47" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C47" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D47" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E47" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="75"/>
-      <c r="B47" s="22" t="s">
+      <c r="F47" s="22"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="87"/>
+      <c r="B48" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="75"/>
-      <c r="B48" s="22" t="s">
-        <v>39</v>
       </c>
       <c r="C48" s="22"/>
       <c r="D48" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="75"/>
+      <c r="A49" s="87"/>
       <c r="B49" s="22" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="87"/>
+      <c r="B50" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E50" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F50" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="78"/>
-      <c r="B50" s="79"/>
-      <c r="C50" s="79"/>
-      <c r="D50" s="79"/>
-      <c r="E50" s="79"/>
-      <c r="F50" s="80"/>
-    </row>
-    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="90"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="F51" s="92"/>
+    </row>
+    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B52" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="27" t="s">
+      <c r="C52" s="26"/>
+      <c r="D52" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E51" s="27" t="s">
+      <c r="E52" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="F51" s="28" t="s">
+      <c r="F52" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="66"/>
-      <c r="B52" s="67"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="68"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="76" t="s">
+    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="55"/>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="57"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B54" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C54" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="30" t="s">
+      <c r="D54" s="29"/>
+      <c r="E54" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F54" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="76"/>
-      <c r="B54" s="29" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="88"/>
+      <c r="B55" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29" t="s">
+      <c r="C55" s="29"/>
+      <c r="D55" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="E55" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F54" s="29"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="76"/>
-      <c r="B55" s="29" t="s">
+      <c r="F55" s="29"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="88"/>
+      <c r="B56" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C56" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="30" t="s">
+      <c r="D56" s="29"/>
+      <c r="E56" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="F56" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="76"/>
-      <c r="B56" s="29" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="88"/>
+      <c r="B57" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="29"/>
-      <c r="D56" s="31" t="s">
+      <c r="C57" s="29"/>
+      <c r="D57" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E56" s="30" t="s">
+      <c r="E57" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F56" s="29"/>
-    </row>
-    <row r="57" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="69"/>
-      <c r="B57" s="70"/>
-      <c r="C57" s="70"/>
-      <c r="D57" s="70"/>
-      <c r="E57" s="70"/>
-      <c r="F57" s="71"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="77" t="s">
+      <c r="F57" s="29"/>
+    </row>
+    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="60"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B59" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C59" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14" t="s">
+      <c r="D59" s="13"/>
+      <c r="E59" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F58" s="13" t="s">
+      <c r="F59" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="77"/>
-      <c r="B59" s="13" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="89"/>
+      <c r="B60" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13" t="s">
+      <c r="C60" s="13"/>
+      <c r="D60" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E60" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F60" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="69"/>
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="71"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="74" t="s">
+    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="58"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="59"/>
+      <c r="F61" s="60"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="15" t="s">
+      <c r="B62" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C62" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="16" t="s">
+      <c r="D62" s="15"/>
+      <c r="E62" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F62" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="74"/>
-      <c r="B62" s="15" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="86"/>
+      <c r="B63" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15" t="s">
+      <c r="C63" s="15"/>
+      <c r="D63" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E63" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F63" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="58" t="s">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="37"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="76" t="s">
         <v>160</v>
       </c>
-      <c r="B64" s="58"/>
-      <c r="C64" s="58"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="58"/>
-    </row>
-    <row r="66" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="73" t="s">
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+    </row>
+    <row r="67" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="B66" s="81"/>
-      <c r="C66" s="81"/>
-      <c r="D66" s="73" t="s">
+      <c r="B67" s="93"/>
+      <c r="C67" s="93"/>
+      <c r="D67" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="73"/>
-    </row>
-    <row r="67" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="87" t="s">
+      <c r="E67" s="85"/>
+    </row>
+    <row r="68" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="88" t="s">
+      <c r="B68" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="C67" s="88" t="s">
+      <c r="C68" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D67" s="40" t="s">
+      <c r="D68" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="E67" s="41" t="s">
+      <c r="E68" s="41" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+    <row r="69" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="39" t="s">
+      <c r="C69" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="89" t="s">
+      <c r="D69" s="98" t="s">
         <v>166</v>
       </c>
-      <c r="E68" s="89" t="s">
+      <c r="E69" s="98" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B70" s="4">
         <v>1</v>
       </c>
-      <c r="C69" s="39" t="s">
+      <c r="C70" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="D69" s="89"/>
-      <c r="E69" s="89"/>
-    </row>
-    <row r="70" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="D70" s="98"/>
+      <c r="E70" s="98"/>
+    </row>
+    <row r="71" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B71" s="5">
         <v>45575.507002314815</v>
       </c>
-      <c r="C70" s="39"/>
-      <c r="D70" s="89"/>
-      <c r="E70" s="89"/>
-    </row>
-    <row r="71" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="C71" s="39"/>
+      <c r="D71" s="98"/>
+      <c r="E71" s="98"/>
+    </row>
+    <row r="72" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C71" s="39" t="s">
+      <c r="C72" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="D71" s="89"/>
-      <c r="E71" s="89"/>
-    </row>
-    <row r="72" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="D72" s="98"/>
+      <c r="E72" s="98"/>
+    </row>
+    <row r="73" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="C73" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="D72" s="89"/>
-      <c r="E72" s="89"/>
-    </row>
-    <row r="73" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="D73" s="98"/>
+      <c r="E73" s="98"/>
+    </row>
+    <row r="74" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="39" t="s">
+      <c r="B74" s="4"/>
+      <c r="C74" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D73" s="89"/>
-      <c r="E73" s="89"/>
-    </row>
-    <row r="74" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="D74" s="98"/>
+      <c r="E74" s="98"/>
+    </row>
+    <row r="75" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B75" s="4">
         <v>11000</v>
       </c>
-      <c r="C74" s="39" t="s">
+      <c r="C75" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="D74" s="89"/>
-      <c r="E74" s="89"/>
-    </row>
-    <row r="75" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="D75" s="98"/>
+      <c r="E75" s="98"/>
+    </row>
+    <row r="76" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B76" s="4">
         <v>100</v>
       </c>
-      <c r="C75" s="39" t="s">
+      <c r="C76" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="D75" s="89"/>
-      <c r="E75" s="89"/>
-    </row>
-    <row r="76" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="D76" s="98"/>
+      <c r="E76" s="98"/>
+    </row>
+    <row r="77" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B77" s="4">
         <v>110</v>
       </c>
-      <c r="C76" s="39" t="s">
+      <c r="C77" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D76" s="89"/>
-      <c r="E76" s="89"/>
-    </row>
-    <row r="77" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="D77" s="98"/>
+      <c r="E77" s="98"/>
+    </row>
+    <row r="78" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B78" s="4">
         <v>11</v>
       </c>
-      <c r="C77" s="39" t="s">
+      <c r="C78" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D77" s="89"/>
-      <c r="E77" s="89"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="49" t="s">
+      <c r="D78" s="98"/>
+      <c r="E78" s="98"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="96" t="s">
         <v>131</v>
       </c>
-      <c r="B78" s="85" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" s="86"/>
-      <c r="D78" s="89"/>
-      <c r="E78" s="89"/>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="50"/>
       <c r="B79" s="83" t="s">
+        <v>210</v>
+      </c>
+      <c r="C79" s="84"/>
+      <c r="D79" s="98"/>
+      <c r="E79" s="98"/>
+    </row>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="97"/>
+      <c r="B80" s="81" t="s">
         <v>134</v>
       </c>
-      <c r="C79" s="84"/>
-      <c r="D79" s="89"/>
-      <c r="E79" s="89"/>
-    </row>
-    <row r="80" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="C80" s="82"/>
+      <c r="D80" s="98"/>
+      <c r="E80" s="98"/>
+    </row>
+    <row r="81" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C80" s="39" t="s">
+      <c r="C81" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D80" s="89"/>
-      <c r="E80" s="89"/>
-    </row>
-    <row r="81" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C81" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D81" s="89"/>
-      <c r="E81" s="89"/>
+      <c r="D81" s="98"/>
+      <c r="E81" s="98"/>
     </row>
     <row r="82" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C82" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D82" s="98"/>
+      <c r="E82" s="98"/>
+    </row>
+    <row r="83" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B83" s="4">
         <v>6</v>
       </c>
-      <c r="C82" s="39" t="s">
+      <c r="C83" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="D82" s="89"/>
-      <c r="E82" s="89"/>
-    </row>
-    <row r="83" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="D83" s="98"/>
+      <c r="E83" s="98"/>
+    </row>
+    <row r="84" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B84" s="4">
         <v>10</v>
       </c>
-      <c r="C83" s="39" t="s">
+      <c r="C84" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="D83" s="89"/>
-      <c r="E83" s="89"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D84" s="38"/>
-      <c r="E84" s="38"/>
+      <c r="D84" s="98"/>
+      <c r="E84" s="98"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D85" s="38"/>
@@ -3454,35 +3581,42 @@
       <c r="D88" s="38"/>
       <c r="E88" s="38"/>
     </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D89" s="38"/>
+      <c r="E89" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="30">
+    <mergeCell ref="B80:C80"/>
     <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="D69:D84"/>
+    <mergeCell ref="E69:E84"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A42:F42"/>
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="D68:D83"/>
-    <mergeCell ref="E68:E83"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C13:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update lisence cmd in xle file
</commit_message>
<xml_diff>
--- a/doc/CMD list of Face attendence .xlsx
+++ b/doc/CMD list of Face attendence .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10598126-CF68-49A6-B2CE-4CC726A9F34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A45C4C-B798-45FB-8577-DD56E33B6356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="224">
   <si>
     <t>ping</t>
   </si>
@@ -1478,6 +1478,27 @@
       <t xml:space="preserve">
 it's also incrimented by 1 for each transection.</t>
     </r>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>subcr&lt;space&gt;0/1</t>
+  </si>
+  <si>
+    <t>73 75 62 63 72 20 00/01</t>
+  </si>
+  <si>
+    <t>ACK</t>
+  </si>
+  <si>
+    <t>ASU</t>
+  </si>
+  <si>
+    <t>41 53 55</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1987,6 +2008,96 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2029,95 +2140,11 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2462,10 +2489,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N89"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2487,28 +2514,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="82" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="78"/>
+      <c r="B4" s="83"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -2539,27 +2566,27 @@
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="61" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
     </row>
     <row r="10" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="84" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="51" t="s">
@@ -2585,11 +2612,11 @@
       <c r="B13" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="66"/>
+      <c r="C13" s="96"/>
       <c r="D13" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="93" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2600,11 +2627,11 @@
       <c r="B14" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="68"/>
+      <c r="C14" s="98"/>
       <c r="D14" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="64"/>
+      <c r="E14" s="94"/>
     </row>
     <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
@@ -2613,11 +2640,11 @@
       <c r="B15" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="98"/>
       <c r="D15" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="E15" s="64"/>
+      <c r="E15" s="94"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
@@ -2626,11 +2653,11 @@
       <c r="B16" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="68"/>
+      <c r="C16" s="98"/>
       <c r="D16" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="E16" s="64"/>
+      <c r="E16" s="94"/>
     </row>
     <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
@@ -2639,11 +2666,11 @@
       <c r="B17" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C17" s="68"/>
+      <c r="C17" s="98"/>
       <c r="D17" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="E17" s="64"/>
+      <c r="E17" s="94"/>
     </row>
     <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
@@ -2652,24 +2679,24 @@
       <c r="B18" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C18" s="67"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E18" s="65"/>
+      <c r="E18" s="95"/>
     </row>
     <row r="19" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="66"/>
+      <c r="B19" s="96"/>
       <c r="C19" s="53" t="s">
         <v>212</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="91" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2677,24 +2704,24 @@
       <c r="A20" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="97"/>
       <c r="C20" s="54" t="s">
         <v>204</v>
       </c>
       <c r="D20" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E20" s="62"/>
+      <c r="E20" s="92"/>
     </row>
     <row r="22" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="80"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
     </row>
     <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="46" t="s">
@@ -2720,7 +2747,7 @@
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="70" t="s">
         <v>128</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -2741,7 +2768,7 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="94"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="9" t="s">
         <v>6</v>
       </c>
@@ -2758,7 +2785,7 @@
       <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="9" t="s">
         <v>107</v>
       </c>
@@ -2773,7 +2800,7 @@
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="94"/>
+      <c r="A27" s="70"/>
       <c r="B27" s="10" t="s">
         <v>30</v>
       </c>
@@ -2790,7 +2817,7 @@
       <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="94"/>
+      <c r="A28" s="70"/>
       <c r="B28" s="10" t="s">
         <v>31</v>
       </c>
@@ -2807,7 +2834,7 @@
       <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="94"/>
+      <c r="A29" s="70"/>
       <c r="B29" s="9" t="s">
         <v>98</v>
       </c>
@@ -2822,7 +2849,7 @@
       <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
+      <c r="A30" s="70"/>
       <c r="B30" s="9" t="s">
         <v>100</v>
       </c>
@@ -2837,7 +2864,7 @@
       <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="94"/>
+      <c r="A31" s="70"/>
       <c r="B31" s="9" t="s">
         <v>103</v>
       </c>
@@ -2852,7 +2879,7 @@
       <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="94"/>
+      <c r="A32" s="70"/>
       <c r="B32" s="9" t="s">
         <v>7</v>
       </c>
@@ -2869,7 +2896,7 @@
       <c r="G32" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
+      <c r="A33" s="70"/>
       <c r="B33" s="9" t="s">
         <v>25</v>
       </c>
@@ -2886,7 +2913,7 @@
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="94"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="9" t="s">
         <v>8</v>
       </c>
@@ -2903,16 +2930,16 @@
       <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="72"/>
+      <c r="A35" s="76"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="78"/>
       <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="95" t="s">
+      <c r="A36" s="71" t="s">
         <v>127</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -2933,7 +2960,7 @@
       <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="95"/>
+      <c r="A37" s="71"/>
       <c r="B37" s="7" t="s">
         <v>9</v>
       </c>
@@ -2950,7 +2977,7 @@
       <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="95"/>
+      <c r="A38" s="71"/>
       <c r="B38" s="7" t="s">
         <v>10</v>
       </c>
@@ -2967,7 +2994,7 @@
       <c r="G38" s="6"/>
     </row>
     <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="95"/>
+      <c r="A39" s="71"/>
       <c r="B39" s="8" t="s">
         <v>20</v>
       </c>
@@ -2984,12 +3011,12 @@
       <c r="G39" s="6"/>
     </row>
     <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="70"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="71"/>
-      <c r="D40" s="71"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="72"/>
+      <c r="A40" s="76"/>
+      <c r="B40" s="77"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="78"/>
       <c r="G40" s="6"/>
     </row>
     <row r="41" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3012,15 +3039,15 @@
       <c r="G41" s="6"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="73"/>
-      <c r="B42" s="74"/>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="75"/>
+      <c r="A42" s="79"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="81"/>
     </row>
     <row r="43" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="87" t="s">
+      <c r="A43" s="63" t="s">
         <v>32</v>
       </c>
       <c r="B43" s="20" t="s">
@@ -3036,7 +3063,7 @@
       <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="87"/>
+      <c r="A44" s="63"/>
       <c r="B44" s="22" t="s">
         <v>36</v>
       </c>
@@ -3050,7 +3077,7 @@
       <c r="F44" s="22"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="87"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="22" t="s">
         <v>109</v>
       </c>
@@ -3064,7 +3091,7 @@
       <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="87"/>
+      <c r="A46" s="63"/>
       <c r="B46" s="22" t="s">
         <v>111</v>
       </c>
@@ -3078,7 +3105,7 @@
       <c r="F46" s="22"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="87"/>
+      <c r="A47" s="63"/>
       <c r="B47" s="22" t="s">
         <v>34</v>
       </c>
@@ -3094,7 +3121,7 @@
       <c r="F47" s="22"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="87"/>
+      <c r="A48" s="63"/>
       <c r="B48" s="22" t="s">
         <v>35</v>
       </c>
@@ -3110,7 +3137,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="87"/>
+      <c r="A49" s="63"/>
       <c r="B49" s="22" t="s">
         <v>39</v>
       </c>
@@ -3126,7 +3153,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="87"/>
+      <c r="A50" s="63"/>
       <c r="B50" s="22" t="s">
         <v>51</v>
       </c>
@@ -3142,12 +3169,12 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="90"/>
-      <c r="B51" s="91"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="92"/>
+      <c r="A51" s="66"/>
+      <c r="B51" s="67"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="68"/>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
@@ -3168,15 +3195,15 @@
       </c>
     </row>
     <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="55"/>
-      <c r="B53" s="56"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="57"/>
+      <c r="A53" s="85"/>
+      <c r="B53" s="86"/>
+      <c r="C53" s="86"/>
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="87"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="88" t="s">
+      <c r="A54" s="64" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="29" t="s">
@@ -3194,7 +3221,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="88"/>
+      <c r="A55" s="64"/>
       <c r="B55" s="29" t="s">
         <v>92</v>
       </c>
@@ -3208,7 +3235,7 @@
       <c r="F55" s="29"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="88"/>
+      <c r="A56" s="64"/>
       <c r="B56" s="29" t="s">
         <v>53</v>
       </c>
@@ -3224,7 +3251,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="88"/>
+      <c r="A57" s="64"/>
       <c r="B57" s="29" t="s">
         <v>92</v>
       </c>
@@ -3237,345 +3264,371 @@
       </c>
       <c r="F57" s="29"/>
     </row>
-    <row r="58" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="58"/>
-      <c r="B58" s="59"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
-      <c r="E58" s="59"/>
-      <c r="F58" s="60"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="88"/>
+      <c r="B58" s="89"/>
+      <c r="C58" s="89"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="90"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="89" t="s">
+      <c r="A59" s="99" t="s">
+        <v>217</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="D59" s="31"/>
+      <c r="E59" s="30" t="s">
+        <v>220</v>
+      </c>
+      <c r="F59" s="29"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="100"/>
+      <c r="B60" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="C60" s="29"/>
+      <c r="D60" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="E60" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="F60" s="29"/>
+    </row>
+    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="88"/>
+      <c r="B61" s="89"/>
+      <c r="C61" s="89"/>
+      <c r="D61" s="89"/>
+      <c r="E61" s="89"/>
+      <c r="F61" s="90"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B62" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C62" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D59" s="13"/>
-      <c r="E59" s="14" t="s">
+      <c r="D62" s="13"/>
+      <c r="E62" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F62" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="89"/>
-      <c r="B60" s="13" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="65"/>
+      <c r="B63" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13" t="s">
+      <c r="C63" s="13"/>
+      <c r="D63" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E63" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F63" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="58"/>
-      <c r="B61" s="59"/>
-      <c r="C61" s="59"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="59"/>
-      <c r="F61" s="60"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="86" t="s">
+    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="88"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="90"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B65" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C65" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D62" s="15"/>
-      <c r="E62" s="16" t="s">
+      <c r="D65" s="15"/>
+      <c r="E65" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F65" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="86"/>
-      <c r="B63" s="15" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="62"/>
+      <c r="B66" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15" t="s">
+      <c r="C66" s="15"/>
+      <c r="D66" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E66" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="F66" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
-      <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="76" t="s">
+    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="37"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="B65" s="76"/>
-      <c r="C65" s="76"/>
-      <c r="D65" s="76"/>
-      <c r="E65" s="76"/>
-      <c r="F65" s="76"/>
-    </row>
-    <row r="67" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="85" t="s">
+      <c r="B68" s="61"/>
+      <c r="C68" s="61"/>
+      <c r="D68" s="61"/>
+      <c r="E68" s="61"/>
+      <c r="F68" s="61"/>
+    </row>
+    <row r="70" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="B67" s="93"/>
-      <c r="C67" s="93"/>
-      <c r="D67" s="85" t="s">
+      <c r="B70" s="69"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="E67" s="85"/>
-    </row>
-    <row r="68" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="47" t="s">
+      <c r="E70" s="60"/>
+    </row>
+    <row r="71" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B68" s="48" t="s">
+      <c r="B71" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="C68" s="48" t="s">
+      <c r="C71" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D68" s="40" t="s">
+      <c r="D71" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="E68" s="41" t="s">
+      <c r="E71" s="41" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="72" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="39" t="s">
+      <c r="C72" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="D69" s="98" t="s">
+      <c r="D72" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="E69" s="98" t="s">
+      <c r="E72" s="74" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+    <row r="73" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B73" s="4">
         <v>1</v>
       </c>
-      <c r="C70" s="39" t="s">
+      <c r="C73" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="D70" s="98"/>
-      <c r="E70" s="98"/>
-    </row>
-    <row r="71" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="D73" s="74"/>
+      <c r="E73" s="74"/>
+    </row>
+    <row r="74" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B74" s="5">
         <v>45575.507002314815</v>
       </c>
-      <c r="C71" s="39"/>
-      <c r="D71" s="98"/>
-      <c r="E71" s="98"/>
-    </row>
-    <row r="72" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="C74" s="39"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+    </row>
+    <row r="75" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="C75" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="D72" s="98"/>
-      <c r="E72" s="98"/>
-    </row>
-    <row r="73" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="D75" s="74"/>
+      <c r="E75" s="74"/>
+    </row>
+    <row r="76" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C73" s="39" t="s">
+      <c r="C76" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="D73" s="98"/>
-      <c r="E73" s="98"/>
-    </row>
-    <row r="74" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="D76" s="74"/>
+      <c r="E76" s="74"/>
+    </row>
+    <row r="77" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="39" t="s">
+      <c r="B77" s="4"/>
+      <c r="C77" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D74" s="98"/>
-      <c r="E74" s="98"/>
-    </row>
-    <row r="75" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+    </row>
+    <row r="78" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B78" s="4">
         <v>11000</v>
       </c>
-      <c r="C75" s="39" t="s">
+      <c r="C78" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="D75" s="98"/>
-      <c r="E75" s="98"/>
-    </row>
-    <row r="76" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="D78" s="74"/>
+      <c r="E78" s="74"/>
+    </row>
+    <row r="79" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B79" s="4">
         <v>100</v>
       </c>
-      <c r="C76" s="39" t="s">
+      <c r="C79" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="D76" s="98"/>
-      <c r="E76" s="98"/>
-    </row>
-    <row r="77" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="D79" s="74"/>
+      <c r="E79" s="74"/>
+    </row>
+    <row r="80" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B80" s="4">
         <v>110</v>
       </c>
-      <c r="C77" s="39" t="s">
+      <c r="C80" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D77" s="98"/>
-      <c r="E77" s="98"/>
-    </row>
-    <row r="78" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+    </row>
+    <row r="81" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B81" s="4">
         <v>11</v>
       </c>
-      <c r="C78" s="39" t="s">
+      <c r="C81" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D78" s="98"/>
-      <c r="E78" s="98"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="96" t="s">
+      <c r="D81" s="74"/>
+      <c r="E81" s="74"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="B79" s="83" t="s">
+      <c r="B82" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="C79" s="84"/>
-      <c r="D79" s="98"/>
-      <c r="E79" s="98"/>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="97"/>
-      <c r="B80" s="81" t="s">
+      <c r="C82" s="58"/>
+      <c r="D82" s="74"/>
+      <c r="E82" s="74"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="73"/>
+      <c r="B83" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C80" s="82"/>
-      <c r="D80" s="98"/>
-      <c r="E80" s="98"/>
-    </row>
-    <row r="81" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="C83" s="56"/>
+      <c r="D83" s="74"/>
+      <c r="E83" s="74"/>
+    </row>
+    <row r="84" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C81" s="39" t="s">
+      <c r="C84" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D81" s="98"/>
-      <c r="E81" s="98"/>
-    </row>
-    <row r="82" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="D84" s="74"/>
+      <c r="E84" s="74"/>
+    </row>
+    <row r="85" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B85" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C82" s="39" t="s">
+      <c r="C85" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="D82" s="98"/>
-      <c r="E82" s="98"/>
-    </row>
-    <row r="83" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="D85" s="74"/>
+      <c r="E85" s="74"/>
+    </row>
+    <row r="86" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B86" s="4">
         <v>6</v>
       </c>
-      <c r="C83" s="39" t="s">
+      <c r="C86" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="D83" s="98"/>
-      <c r="E83" s="98"/>
-    </row>
-    <row r="84" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="D86" s="74"/>
+      <c r="E86" s="74"/>
+    </row>
+    <row r="87" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B87" s="4">
         <v>10</v>
       </c>
-      <c r="C84" s="39" t="s">
+      <c r="C87" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="D84" s="98"/>
-      <c r="E84" s="98"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
+      <c r="D87" s="74"/>
+      <c r="E87" s="74"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D88" s="38"/>
@@ -3585,24 +3638,29 @@
       <c r="D89" s="38"/>
       <c r="E89" s="38"/>
     </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D90" s="38"/>
+      <c r="E90" s="38"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A54:A57"/>
+  <mergeCells count="32">
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A64:F64"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E13:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="A58:F58"/>
     <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="D69:D84"/>
-    <mergeCell ref="E69:E84"/>
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A35:F35"/>
     <mergeCell ref="A40:F40"/>
@@ -3610,13 +3668,22 @@
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C13:C18"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A43:A50"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="D72:D87"/>
+    <mergeCell ref="E72:E87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add wss custom pac in excle
</commit_message>
<xml_diff>
--- a/doc/CMD list of Face attendence .xlsx
+++ b/doc/CMD list of Face attendence .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A45C4C-B798-45FB-8577-DD56E33B6356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16389218-72CC-4A46-AF6E-8157E44A4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$23:$F$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$50:$F$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="239">
   <si>
     <t>ping</t>
   </si>
@@ -1500,12 +1500,74 @@
   <si>
     <t>41 53 55</t>
   </si>
+  <si>
+    <t>4 byte version id + unique ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end packet </t>
+  </si>
+  <si>
+    <t>Device type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSS Custom Protocall </t>
+  </si>
+  <si>
+    <t>ID:</t>
+  </si>
+  <si>
+    <t>DEVICE_VERSION_ID=AA00 , uniqueID = 242829063</t>
+  </si>
+  <si>
+    <t>Data Type B means Binary</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data  = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>31 32 33 34</t>
+    </r>
+  </si>
+  <si>
+    <t>44 45 56 49 43 45 5F 54 59 50 45 3A 55 46 41 43 45 5C 6E</t>
+  </si>
+  <si>
+    <t>44 41 54 41 5F 54 59 50 45 3A 42 5C 6E</t>
+  </si>
+  <si>
+    <t>49 44 3a + 41 41 30 30 + 32 34 32 38 32 39 30 36 33 + 5c 6e</t>
+  </si>
+  <si>
+    <t>Hex Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44 41 54 41 3A + 31 32 33 34 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5C 6E 5C 6E 5C 75 30 30 30 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEVICE_TYPE:UFACE\n
+ID:DEVICE_VERSION_ID+uniqueID\n
+DATA_TYPE:B\n
+DATA: binary data
+\n\n\u0000
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1628,6 +1690,27 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="0.79998168889431442"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1890,7 +1973,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2008,6 +2091,90 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2020,15 +2187,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2068,83 +2229,88 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2489,10 +2655,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N92"/>
+  <dimension ref="A1:N119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,28 +2680,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="71" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="83"/>
+      <c r="B4" s="80"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -2562,1128 +2728,1363 @@
       </c>
     </row>
     <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+      <c r="A8" s="101"/>
+      <c r="B8" s="101"/>
+    </row>
+    <row r="9" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="80"/>
+      <c r="C9" s="104" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" s="104" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" s="116"/>
+    </row>
+    <row r="10" spans="1:6" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="119" t="s">
+        <v>238</v>
+      </c>
+      <c r="B10" s="119"/>
+      <c r="C10" s="111" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" s="105" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="117"/>
+    </row>
+    <row r="11" spans="1:6" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="119"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="110" t="s">
+        <v>234</v>
+      </c>
+      <c r="D11" s="106" t="s">
+        <v>224</v>
+      </c>
+      <c r="E11" s="117"/>
+    </row>
+    <row r="12" spans="1:6" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="119"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="112" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="113" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="117"/>
+    </row>
+    <row r="13" spans="1:6" s="42" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="119"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="114" t="s">
+        <v>236</v>
+      </c>
+      <c r="D13" s="107" t="s">
+        <v>231</v>
+      </c>
+      <c r="E13" s="117"/>
+    </row>
+    <row r="14" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="119"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="115" t="s">
+        <v>237</v>
+      </c>
+      <c r="D14" s="108" t="s">
+        <v>225</v>
+      </c>
+      <c r="E14" s="117"/>
+    </row>
+    <row r="15" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="120"/>
+      <c r="B15" s="120"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="117"/>
+    </row>
+    <row r="16" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="87" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="87"/>
+    </row>
+    <row r="17" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D18" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="E18" s="100" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+    </row>
+    <row r="20" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="5">
+        <v>45575.507002314815</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="100"/>
+    </row>
+    <row r="21" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+    </row>
+    <row r="22" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="100"/>
+      <c r="E22" s="100"/>
+    </row>
+    <row r="23" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="100"/>
+      <c r="E23" s="100"/>
+    </row>
+    <row r="24" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="4">
+        <v>11000</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+    </row>
+    <row r="25" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="4">
+        <v>100</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+    </row>
+    <row r="26" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="4">
+        <v>110</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+    </row>
+    <row r="27" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="4">
+        <v>11</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="100"/>
+      <c r="E27" s="100"/>
+    </row>
+    <row r="28" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="98" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="85" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" s="86"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="100"/>
+    </row>
+    <row r="29" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="99"/>
+      <c r="B29" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" s="84"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="100"/>
+    </row>
+    <row r="30" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="100"/>
+      <c r="E30" s="100"/>
+    </row>
+    <row r="31" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+    </row>
+    <row r="32" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="4">
+        <v>6</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="100"/>
+      <c r="E32" s="100"/>
+    </row>
+    <row r="33" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="4">
+        <v>10</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+    </row>
+    <row r="34" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="109" t="s">
+        <v>229</v>
+      </c>
+      <c r="C34" s="109"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+    </row>
+    <row r="35" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="120"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="117"/>
+    </row>
+    <row r="36" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-    </row>
-    <row r="10" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="84" t="s">
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+    </row>
+    <row r="37" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="81" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+    </row>
+    <row r="39" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B39" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C39" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D39" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E39" s="33" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+    <row r="40" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B40" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="36" t="s">
+      <c r="C40" s="66"/>
+      <c r="D40" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="E13" s="93" t="s">
+      <c r="E40" s="63" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
+    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B41" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="36" t="s">
+      <c r="C41" s="68"/>
+      <c r="D41" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="E14" s="94"/>
-    </row>
-    <row r="15" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="E41" s="64"/>
+    </row>
+    <row r="42" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B42" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="98"/>
-      <c r="D15" s="36" t="s">
+      <c r="C42" s="68"/>
+      <c r="D42" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="E15" s="94"/>
-    </row>
-    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
+      <c r="E42" s="64"/>
+    </row>
+    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B43" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="36" t="s">
+      <c r="C43" s="68"/>
+      <c r="D43" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="E16" s="94"/>
-    </row>
-    <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="E43" s="64"/>
+    </row>
+    <row r="44" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B44" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="36" t="s">
+      <c r="C44" s="68"/>
+      <c r="D44" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="E17" s="94"/>
-    </row>
-    <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
+      <c r="E44" s="64"/>
+    </row>
+    <row r="45" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="52" t="s">
         <v>207</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B45" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C18" s="97"/>
-      <c r="D18" s="36" t="s">
+      <c r="C45" s="67"/>
+      <c r="D45" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E18" s="95"/>
-    </row>
-    <row r="19" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
+      <c r="E45" s="65"/>
+    </row>
+    <row r="46" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B19" s="96"/>
-      <c r="C19" s="53" t="s">
+      <c r="B46" s="66"/>
+      <c r="C46" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D46" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="E19" s="91" t="s">
+      <c r="E46" s="61" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B20" s="97"/>
-      <c r="C20" s="54" t="s">
+      <c r="B47" s="67"/>
+      <c r="C47" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D47" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E20" s="92"/>
-    </row>
-    <row r="22" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="E47" s="62"/>
+    </row>
+    <row r="49" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="82" t="s">
         <v>178</v>
       </c>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-    </row>
-    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="46" t="s">
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+    </row>
+    <row r="50" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A50" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B50" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C50" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="46" t="s">
+      <c r="D50" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="46" t="s">
+      <c r="E50" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="F23" s="46" t="s">
+      <c r="F50" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="70" t="s">
+      <c r="G50" s="6"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+    </row>
+    <row r="51" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B51" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C51" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F51" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70"/>
-      <c r="B25" s="9" t="s">
+      <c r="G51" s="6"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+    </row>
+    <row r="52" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="96"/>
+      <c r="B52" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9" t="s">
+      <c r="C52" s="9"/>
+      <c r="D52" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E52" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F52" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
-      <c r="B26" s="9" t="s">
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="96"/>
+      <c r="B53" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10" t="s">
+      <c r="D53" s="9"/>
+      <c r="E53" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="70"/>
-      <c r="B27" s="10" t="s">
+      <c r="F53" s="12"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="96"/>
+      <c r="B54" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="11" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F54" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
-      <c r="B28" s="10" t="s">
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="96"/>
+      <c r="B55" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="11" t="s">
+      <c r="C55" s="9"/>
+      <c r="D55" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E55" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
-      <c r="B29" s="9" t="s">
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="96"/>
+      <c r="B56" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C56" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9" t="s">
+      <c r="D56" s="9"/>
+      <c r="E56" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="70"/>
-      <c r="B30" s="9" t="s">
+      <c r="F56" s="9"/>
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="96"/>
+      <c r="B57" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E57" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="70"/>
-      <c r="B31" s="9" t="s">
+      <c r="F57" s="9"/>
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="96"/>
+      <c r="B58" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E58" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="70"/>
-      <c r="B32" s="9" t="s">
+      <c r="F58" s="9"/>
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="96"/>
+      <c r="B59" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="s">
+      <c r="C59" s="9"/>
+      <c r="D59" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E59" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F59" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="70"/>
-      <c r="B33" s="9" t="s">
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="96"/>
+      <c r="B60" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E60" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F60" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="70"/>
-      <c r="B34" s="9" t="s">
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="96"/>
+      <c r="B61" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
+      <c r="C61" s="9"/>
+      <c r="D61" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E61" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F61" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="76"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="71" t="s">
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="72"/>
+      <c r="B62" s="73"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
+      <c r="F62" s="74"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="97" t="s">
         <v>127</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B63" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
-      <c r="B37" s="7" t="s">
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="97"/>
+      <c r="B64" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7" t="s">
+      <c r="C64" s="7"/>
+      <c r="D64" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F64" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
-      <c r="B38" s="7" t="s">
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="97"/>
+      <c r="B65" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
+      <c r="C65" s="7"/>
+      <c r="D65" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
-      <c r="B39" s="8" t="s">
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="97"/>
+      <c r="B66" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8" t="s">
+      <c r="C66" s="7"/>
+      <c r="D66" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="72"/>
+      <c r="B67" s="73"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="73"/>
+      <c r="E67" s="73"/>
+      <c r="F67" s="74"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B68" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="17" t="s">
+      <c r="C68" s="14"/>
+      <c r="D68" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E68" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="F68" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="79"/>
-      <c r="B42" s="80"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="81"/>
-    </row>
-    <row r="43" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="63" t="s">
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="75"/>
+      <c r="B69" s="76"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="77"/>
+    </row>
+    <row r="70" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B70" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C70" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D43" s="22"/>
-      <c r="E43" s="23" t="s">
+      <c r="D70" s="22"/>
+      <c r="E70" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="63"/>
-      <c r="B44" s="22" t="s">
+      <c r="F70" s="22"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="89"/>
+      <c r="B71" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22" t="s">
+      <c r="C71" s="22"/>
+      <c r="D71" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E71" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
-      <c r="B45" s="22" t="s">
+      <c r="F71" s="22"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="89"/>
+      <c r="B72" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="32" t="s">
+      <c r="C72" s="22"/>
+      <c r="D72" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E72" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
-      <c r="B46" s="22" t="s">
+      <c r="F72" s="22"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="89"/>
+      <c r="B73" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="32" t="s">
+      <c r="C73" s="22"/>
+      <c r="D73" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E73" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="63"/>
-      <c r="B47" s="22" t="s">
+      <c r="F73" s="22"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="89"/>
+      <c r="B74" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="E47" s="24" t="s">
+      <c r="E74" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="F47" s="22"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="63"/>
-      <c r="B48" s="22" t="s">
+      <c r="F74" s="22"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="89"/>
+      <c r="B75" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22" t="s">
+      <c r="C75" s="22"/>
+      <c r="D75" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E75" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F75" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
-      <c r="B49" s="22" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="89"/>
+      <c r="B76" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22" t="s">
+      <c r="C76" s="22"/>
+      <c r="D76" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E76" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F76" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="63"/>
-      <c r="B50" s="22" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="89"/>
+      <c r="B77" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="22" t="s">
+      <c r="C77" s="22"/>
+      <c r="D77" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E77" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F77" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="66"/>
-      <c r="B51" s="67"/>
-      <c r="C51" s="67"/>
-      <c r="D51" s="67"/>
-      <c r="E51" s="67"/>
-      <c r="F51" s="68"/>
-    </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="92"/>
+      <c r="B78" s="93"/>
+      <c r="C78" s="93"/>
+      <c r="D78" s="93"/>
+      <c r="E78" s="93"/>
+      <c r="F78" s="94"/>
+    </row>
+    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="27" t="s">
+      <c r="B79" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="27" t="s">
+      <c r="C79" s="26"/>
+      <c r="D79" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E52" s="27" t="s">
+      <c r="E79" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="F52" s="28" t="s">
+      <c r="F79" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="85"/>
-      <c r="B53" s="86"/>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="87"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="64" t="s">
+    <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="55"/>
+      <c r="B80" s="56"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="56"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="57"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B81" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="29" t="s">
+      <c r="C81" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30" t="s">
+      <c r="D81" s="29"/>
+      <c r="E81" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F81" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="64"/>
-      <c r="B55" s="29" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="90"/>
+      <c r="B82" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29" t="s">
+      <c r="C82" s="29"/>
+      <c r="D82" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E82" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F55" s="29"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="64"/>
-      <c r="B56" s="29" t="s">
+      <c r="F82" s="29"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="90"/>
+      <c r="B83" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="29" t="s">
+      <c r="C83" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="30" t="s">
+      <c r="D83" s="29"/>
+      <c r="E83" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F83" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="64"/>
-      <c r="B57" s="29" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="90"/>
+      <c r="B84" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="29"/>
-      <c r="D57" s="31" t="s">
+      <c r="C84" s="29"/>
+      <c r="D84" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="E84" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F57" s="29"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="88"/>
-      <c r="B58" s="89"/>
-      <c r="C58" s="89"/>
-      <c r="D58" s="89"/>
-      <c r="E58" s="89"/>
-      <c r="F58" s="90"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="99" t="s">
+      <c r="F84" s="29"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="58"/>
+      <c r="B85" s="59"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="59"/>
+      <c r="E85" s="59"/>
+      <c r="F85" s="60"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="69" t="s">
         <v>217</v>
       </c>
-      <c r="B59" s="29" t="s">
+      <c r="B86" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C59" s="29" t="s">
+      <c r="C86" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="D59" s="31"/>
-      <c r="E59" s="30" t="s">
+      <c r="D86" s="31"/>
+      <c r="E86" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="F59" s="29"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="100"/>
-      <c r="B60" s="29" t="s">
+      <c r="F86" s="29"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="70"/>
+      <c r="B87" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="31" t="s">
+      <c r="C87" s="29"/>
+      <c r="D87" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="E60" s="30" t="s">
+      <c r="E87" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="F60" s="29"/>
-    </row>
-    <row r="61" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="88"/>
-      <c r="B61" s="89"/>
-      <c r="C61" s="89"/>
-      <c r="D61" s="89"/>
-      <c r="E61" s="89"/>
-      <c r="F61" s="90"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="65" t="s">
+      <c r="F87" s="29"/>
+    </row>
+    <row r="88" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="58"/>
+      <c r="B88" s="59"/>
+      <c r="C88" s="59"/>
+      <c r="D88" s="59"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="60"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="91" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B89" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C89" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D62" s="13"/>
-      <c r="E62" s="14" t="s">
+      <c r="D89" s="13"/>
+      <c r="E89" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F89" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
-      <c r="B63" s="13" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="91"/>
+      <c r="B90" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13" t="s">
+      <c r="C90" s="13"/>
+      <c r="D90" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E90" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F63" s="13" t="s">
+      <c r="F90" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="88"/>
-      <c r="B64" s="89"/>
-      <c r="C64" s="89"/>
-      <c r="D64" s="89"/>
-      <c r="E64" s="89"/>
-      <c r="F64" s="90"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="62" t="s">
+    <row r="91" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="58"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="59"/>
+      <c r="D91" s="59"/>
+      <c r="E91" s="59"/>
+      <c r="F91" s="60"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="15" t="s">
+      <c r="B92" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C92" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D65" s="15"/>
-      <c r="E65" s="16" t="s">
+      <c r="D92" s="15"/>
+      <c r="E92" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F65" s="15" t="s">
+      <c r="F92" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="62"/>
-      <c r="B66" s="15" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="88"/>
+      <c r="B93" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15" t="s">
+      <c r="C93" s="15"/>
+      <c r="D93" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E93" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="15" t="s">
+      <c r="F93" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="61" t="s">
+    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="37"/>
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="B68" s="61"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="61"/>
-    </row>
-    <row r="70" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="B70" s="69"/>
-      <c r="C70" s="69"/>
-      <c r="D70" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="E70" s="60"/>
-    </row>
-    <row r="71" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="B71" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D71" s="40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E71" s="41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D72" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="E72" s="74" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73" s="4">
-        <v>1</v>
-      </c>
-      <c r="C73" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D73" s="74"/>
-      <c r="E73" s="74"/>
-    </row>
-    <row r="74" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="5">
-        <v>45575.507002314815</v>
-      </c>
-      <c r="C74" s="39"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="74"/>
-    </row>
-    <row r="75" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C75" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-    </row>
-    <row r="76" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C76" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-    </row>
-    <row r="77" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D77" s="74"/>
-      <c r="E77" s="74"/>
-    </row>
-    <row r="78" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" s="4">
-        <v>11000</v>
-      </c>
-      <c r="C78" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-    </row>
-    <row r="79" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79" s="4">
-        <v>100</v>
-      </c>
-      <c r="C79" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D79" s="74"/>
-      <c r="E79" s="74"/>
-    </row>
-    <row r="80" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80" s="4">
-        <v>110</v>
-      </c>
-      <c r="C80" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="D80" s="74"/>
-      <c r="E80" s="74"/>
-    </row>
-    <row r="81" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" s="4">
-        <v>11</v>
-      </c>
-      <c r="C81" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D81" s="74"/>
-      <c r="E81" s="74"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="72" t="s">
-        <v>131</v>
-      </c>
-      <c r="B82" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="C82" s="58"/>
-      <c r="D82" s="74"/>
-      <c r="E82" s="74"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="73"/>
-      <c r="B83" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="C83" s="56"/>
-      <c r="D83" s="74"/>
-      <c r="E83" s="74"/>
-    </row>
-    <row r="84" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C84" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D84" s="74"/>
-      <c r="E84" s="74"/>
-    </row>
-    <row r="85" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C85" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D85" s="74"/>
-      <c r="E85" s="74"/>
-    </row>
-    <row r="86" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B86" s="4">
-        <v>6</v>
-      </c>
-      <c r="C86" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-    </row>
-    <row r="87" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B87" s="4">
-        <v>10</v>
-      </c>
-      <c r="C87" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D87" s="74"/>
-      <c r="E87" s="74"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
+      <c r="B95" s="78"/>
+      <c r="C95" s="78"/>
+      <c r="D95" s="78"/>
+      <c r="E95" s="78"/>
+      <c r="F95" s="78"/>
+    </row>
+    <row r="97" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="122"/>
+      <c r="B97" s="123"/>
+      <c r="C97" s="123"/>
+      <c r="D97" s="122"/>
+      <c r="E97" s="122"/>
+    </row>
+    <row r="98" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="124"/>
+      <c r="B98" s="125"/>
+      <c r="C98" s="125"/>
+      <c r="D98" s="126"/>
+      <c r="E98" s="127"/>
+    </row>
+    <row r="99" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="101"/>
+      <c r="B99" s="102"/>
+      <c r="C99" s="102"/>
+      <c r="D99" s="128"/>
+      <c r="E99" s="128"/>
+    </row>
+    <row r="100" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="101"/>
+      <c r="B100" s="102"/>
+      <c r="C100" s="102"/>
+      <c r="D100" s="128"/>
+      <c r="E100" s="128"/>
+    </row>
+    <row r="101" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="101"/>
+      <c r="B101" s="129"/>
+      <c r="C101" s="102"/>
+      <c r="D101" s="128"/>
+      <c r="E101" s="128"/>
+    </row>
+    <row r="102" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="101"/>
+      <c r="B102" s="102"/>
+      <c r="C102" s="102"/>
+      <c r="D102" s="128"/>
+      <c r="E102" s="128"/>
+    </row>
+    <row r="103" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="101"/>
+      <c r="B103" s="102"/>
+      <c r="C103" s="102"/>
+      <c r="D103" s="128"/>
+      <c r="E103" s="128"/>
+    </row>
+    <row r="104" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="101"/>
+      <c r="B104" s="102"/>
+      <c r="C104" s="102"/>
+      <c r="D104" s="128"/>
+      <c r="E104" s="128"/>
+    </row>
+    <row r="105" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="101"/>
+      <c r="B105" s="102"/>
+      <c r="C105" s="102"/>
+      <c r="D105" s="128"/>
+      <c r="E105" s="128"/>
+    </row>
+    <row r="106" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="101"/>
+      <c r="B106" s="102"/>
+      <c r="C106" s="102"/>
+      <c r="D106" s="128"/>
+      <c r="E106" s="128"/>
+    </row>
+    <row r="107" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="101"/>
+      <c r="B107" s="102"/>
+      <c r="C107" s="102"/>
+      <c r="D107" s="128"/>
+      <c r="E107" s="128"/>
+    </row>
+    <row r="108" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="101"/>
+      <c r="B108" s="102"/>
+      <c r="C108" s="102"/>
+      <c r="D108" s="128"/>
+      <c r="E108" s="128"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="130"/>
+      <c r="B109" s="131"/>
+      <c r="C109" s="131"/>
+      <c r="D109" s="128"/>
+      <c r="E109" s="128"/>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="130"/>
+      <c r="B110" s="132"/>
+      <c r="C110" s="132"/>
+      <c r="D110" s="128"/>
+      <c r="E110" s="128"/>
+    </row>
+    <row r="111" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="101"/>
+      <c r="B111" s="102"/>
+      <c r="C111" s="102"/>
+      <c r="D111" s="128"/>
+      <c r="E111" s="128"/>
+    </row>
+    <row r="112" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="101"/>
+      <c r="B112" s="102"/>
+      <c r="C112" s="102"/>
+      <c r="D112" s="128"/>
+      <c r="E112" s="128"/>
+    </row>
+    <row r="113" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="101"/>
+      <c r="B113" s="102"/>
+      <c r="C113" s="102"/>
+      <c r="D113" s="128"/>
+      <c r="E113" s="128"/>
+    </row>
+    <row r="114" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="101"/>
+      <c r="B114" s="102"/>
+      <c r="C114" s="102"/>
+      <c r="D114" s="128"/>
+      <c r="E114" s="128"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="101"/>
+      <c r="B115" s="103"/>
+      <c r="C115" s="103"/>
+      <c r="D115" s="133"/>
+      <c r="E115" s="133"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D117" s="38"/>
+      <c r="E117" s="38"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="38"/>
+      <c r="E118" s="38"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D119" s="38"/>
+      <c r="E119" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E13:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C13:C18"/>
-    <mergeCell ref="A58:F58"/>
-    <mergeCell ref="A59:A60"/>
+  <mergeCells count="43">
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="A10:B14"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D18:D33"/>
+    <mergeCell ref="E18:E33"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="A49:F49"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A95:F95"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A70:A77"/>
+    <mergeCell ref="A81:A84"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A51:A61"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="D99:D114"/>
+    <mergeCell ref="E99:E114"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A40:F40"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A62:F62"/>
+    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A36:F36"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A68:F68"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A43:A50"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A24:A34"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="D72:D87"/>
-    <mergeCell ref="E72:E87"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A88:F88"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="E40:E45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C40:C45"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A86:A87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add service uuid in excle
</commit_message>
<xml_diff>
--- a/doc/CMD list of Face attendence .xlsx
+++ b/doc/CMD list of Face attendence .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16389218-72CC-4A46-AF6E-8157E44A4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FF7388-3D5E-4CB7-9965-1A1EC9FA2164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$50:$F$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$52:$F$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="241">
   <si>
     <t>ping</t>
   </si>
@@ -1561,6 +1561,12 @@
 DATA: binary data
 \n\n\u0000
 </t>
+  </si>
+  <si>
+    <t>SERVICE_UUID</t>
+  </si>
+  <si>
+    <t>0xFFFF</t>
   </si>
 </sst>
 </file>
@@ -1973,7 +1979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2091,6 +2097,175 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2138,179 +2313,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2655,10 +2657,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:N121"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2680,1355 +2682,1356 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="106" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="113" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="80"/>
+      <c r="B4" s="114"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B6" s="35" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+    <row r="7" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B7" s="45" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+    <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B8" s="35" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="101"/>
-      <c r="B8" s="101"/>
-    </row>
-    <row r="9" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="s">
+    <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="113" t="s">
         <v>227</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="104" t="s">
+      <c r="B11" s="114"/>
+      <c r="C11" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="104" t="s">
+      <c r="D11" s="56" t="s">
         <v>168</v>
       </c>
-      <c r="E9" s="116"/>
-    </row>
-    <row r="10" spans="1:6" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="119" t="s">
+      <c r="E11" s="67"/>
+    </row>
+    <row r="12" spans="1:6" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="78" t="s">
         <v>238</v>
       </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="111" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D12" s="57" t="s">
         <v>226</v>
       </c>
-      <c r="E10" s="117"/>
-    </row>
-    <row r="11" spans="1:6" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="119"/>
-      <c r="B11" s="119"/>
-      <c r="C11" s="110" t="s">
+      <c r="E12" s="68"/>
+    </row>
+    <row r="13" spans="1:6" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="61" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="106" t="s">
+      <c r="D13" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="E11" s="117"/>
-    </row>
-    <row r="12" spans="1:6" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="119"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="112" t="s">
+      <c r="E13" s="68"/>
+    </row>
+    <row r="14" spans="1:6" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="D12" s="113" t="s">
+      <c r="D14" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="E12" s="117"/>
-    </row>
-    <row r="13" spans="1:6" s="42" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="119"/>
-      <c r="B13" s="119"/>
-      <c r="C13" s="114" t="s">
+      <c r="E14" s="68"/>
+    </row>
+    <row r="15" spans="1:6" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D15" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="E13" s="117"/>
-    </row>
-    <row r="14" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="119"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="115" t="s">
+      <c r="E15" s="68"/>
+    </row>
+    <row r="16" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="66" t="s">
         <v>237</v>
       </c>
-      <c r="D14" s="108" t="s">
+      <c r="D16" s="60" t="s">
         <v>225</v>
       </c>
-      <c r="E14" s="117"/>
-    </row>
-    <row r="15" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="120"/>
-      <c r="B15" s="120"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="117"/>
-    </row>
-    <row r="16" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="87" t="s">
+      <c r="E16" s="68"/>
+    </row>
+    <row r="17" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="68"/>
+    </row>
+    <row r="18" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="79" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="95"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="87" t="s">
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="E16" s="87"/>
-    </row>
-    <row r="17" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="47" t="s">
+      <c r="E18" s="79"/>
+    </row>
+    <row r="19" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B19" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C19" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D19" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E19" s="41" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" s="100" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" s="100" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
     </row>
     <row r="20" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="5">
-        <v>45575.507002314815</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
+        <v>70</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="81" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="21" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
+        <v>126</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
     </row>
     <row r="22" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="100"/>
-      <c r="E22" s="100"/>
+        <v>72</v>
+      </c>
+      <c r="B22" s="5">
+        <v>45575.507002314815</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="C23" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="100"/>
-      <c r="E23" s="100"/>
+        <v>152</v>
+      </c>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
     </row>
     <row r="24" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="4">
-        <v>11000</v>
+        <v>75</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
+        <v>79</v>
+      </c>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
     </row>
     <row r="25" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="4">
-        <v>100</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="100"/>
-      <c r="E25" s="100"/>
+        <v>77</v>
+      </c>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
     </row>
     <row r="26" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B26" s="4">
-        <v>110</v>
+        <v>11000</v>
       </c>
       <c r="C26" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
+        <v>153</v>
+      </c>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
     </row>
     <row r="27" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="4">
+        <v>100</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+    </row>
+    <row r="28" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="4">
+        <v>110</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="81"/>
+      <c r="E28" s="81"/>
+    </row>
+    <row r="29" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B29" s="4">
         <v>11</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C29" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="100"/>
-      <c r="E27" s="100"/>
-    </row>
-    <row r="28" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="98" t="s">
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+    </row>
+    <row r="30" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="B28" s="85" t="s">
+      <c r="B30" s="84" t="s">
         <v>210</v>
       </c>
-      <c r="C28" s="86"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="100"/>
-    </row>
-    <row r="29" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="99"/>
-      <c r="B29" s="83" t="s">
+      <c r="C30" s="85"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="81"/>
+    </row>
+    <row r="31" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="83"/>
+      <c r="B31" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="84"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="100"/>
-    </row>
-    <row r="30" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="100"/>
-      <c r="E30" s="100"/>
-    </row>
-    <row r="31" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
     </row>
     <row r="32" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B32" s="4">
-        <v>6</v>
+        <v>143</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
+        <v>154</v>
+      </c>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
     </row>
     <row r="33" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" s="4">
-        <v>10</v>
+        <v>145</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
+        <v>155</v>
+      </c>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
     </row>
     <row r="34" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="4">
+        <v>6</v>
+      </c>
+      <c r="C34" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+    </row>
+    <row r="35" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="4">
+        <v>10</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+    </row>
+    <row r="36" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B34" s="109" t="s">
+      <c r="B36" s="88" t="s">
         <v>229</v>
       </c>
-      <c r="C34" s="109"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-    </row>
-    <row r="35" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="120"/>
-      <c r="B35" s="120"/>
-      <c r="C35" s="118"/>
-      <c r="D35" s="121"/>
-      <c r="E35" s="117"/>
-    </row>
-    <row r="36" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78" t="s">
+      <c r="C36" s="88"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+    </row>
+    <row r="37" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="70"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="68"/>
+    </row>
+    <row r="38" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="93" t="s">
         <v>161</v>
       </c>
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="78"/>
-    </row>
-    <row r="37" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="81" t="s">
+      <c r="B38" s="93"/>
+      <c r="C38" s="93"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="93"/>
+    </row>
+    <row r="39" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="115" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-    </row>
-    <row r="39" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51" t="s">
+      <c r="B40" s="91"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="91"/>
+    </row>
+    <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="34" t="s">
+      <c r="B41" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C41" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D41" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E39" s="33" t="s">
+      <c r="E41" s="33" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" s="63" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E41" s="64"/>
     </row>
     <row r="42" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="52" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="C42" s="68"/>
+        <v>199</v>
+      </c>
+      <c r="C42" s="127"/>
       <c r="D42" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E42" s="64"/>
-    </row>
-    <row r="43" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="E42" s="124" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="52" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="C43" s="68"/>
+        <v>200</v>
+      </c>
+      <c r="C43" s="129"/>
       <c r="D43" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="E43" s="64"/>
+        <v>186</v>
+      </c>
+      <c r="E43" s="125"/>
     </row>
     <row r="44" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C44" s="129"/>
+      <c r="D44" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E44" s="125"/>
+    </row>
+    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" s="129"/>
+      <c r="D45" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" s="125"/>
+    </row>
+    <row r="46" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B46" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C44" s="68"/>
-      <c r="D44" s="36" t="s">
+      <c r="C46" s="129"/>
+      <c r="D46" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="64"/>
-    </row>
-    <row r="45" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="52" t="s">
+      <c r="E46" s="125"/>
+    </row>
+    <row r="47" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="52" t="s">
         <v>207</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B47" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C45" s="67"/>
-      <c r="D45" s="36" t="s">
+      <c r="C47" s="128"/>
+      <c r="D47" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E45" s="65"/>
-    </row>
-    <row r="46" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="s">
+      <c r="E47" s="126"/>
+    </row>
+    <row r="48" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B46" s="66"/>
-      <c r="C46" s="53" t="s">
+      <c r="B48" s="127"/>
+      <c r="C48" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="D46" s="50" t="s">
+      <c r="D48" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="E46" s="61" t="s">
+      <c r="E48" s="122" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="43" t="s">
+    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B47" s="67"/>
-      <c r="C47" s="54" t="s">
+      <c r="B49" s="128"/>
+      <c r="C49" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="D47" s="44" t="s">
+      <c r="D49" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E47" s="62"/>
-    </row>
-    <row r="49" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="82" t="s">
+      <c r="E49" s="123"/>
+    </row>
+    <row r="51" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="91" t="s">
         <v>178</v>
       </c>
-      <c r="B49" s="82"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-    </row>
-    <row r="50" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A50" s="46" t="s">
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="F51" s="91"/>
+    </row>
+    <row r="52" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A52" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="B50" s="46" t="s">
+      <c r="B52" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="46" t="s">
+      <c r="C52" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="46" t="s">
+      <c r="D52" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E50" s="46" t="s">
+      <c r="E52" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="F50" s="46" t="s">
+      <c r="F52" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="G50" s="6"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="96" t="s">
+      <c r="G52" s="6"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+    </row>
+    <row r="53" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="102" t="s">
         <v>128</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B53" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10" t="s">
+      <c r="D53" s="10"/>
+      <c r="E53" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G51" s="6"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="96"/>
-      <c r="B52" s="9" t="s">
+      <c r="G53" s="6"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+    </row>
+    <row r="54" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="102"/>
+      <c r="B54" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E54" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F54" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G52" s="6"/>
-    </row>
-    <row r="53" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="96"/>
-      <c r="B53" s="9" t="s">
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="102"/>
+      <c r="B55" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C55" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="9"/>
-      <c r="E53" s="10" t="s">
+      <c r="D55" s="9"/>
+      <c r="E55" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="6"/>
-    </row>
-    <row r="54" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="96"/>
-      <c r="B54" s="10" t="s">
+      <c r="F55" s="12"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="102"/>
+      <c r="B56" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="11" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E56" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F56" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="96"/>
-      <c r="B55" s="10" t="s">
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="102"/>
+      <c r="B57" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="11" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="E57" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F57" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G55" s="6"/>
-    </row>
-    <row r="56" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="96"/>
-      <c r="B56" s="9" t="s">
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="102"/>
+      <c r="B58" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C58" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9" t="s">
+      <c r="D58" s="9"/>
+      <c r="E58" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="F56" s="9"/>
-      <c r="G56" s="6"/>
-    </row>
-    <row r="57" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="96"/>
-      <c r="B57" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="6"/>
-    </row>
-    <row r="58" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="96"/>
-      <c r="B58" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="96"/>
+    <row r="59" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="102"/>
       <c r="B59" s="9" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="9" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="F59" s="9"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="96"/>
+    <row r="60" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="102"/>
       <c r="B60" s="9" t="s">
-        <v>25</v>
+        <v>103</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="9" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F60" s="9"/>
       <c r="G60" s="6"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="96"/>
+      <c r="A61" s="102"/>
       <c r="B61" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="102"/>
+      <c r="B62" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="102"/>
+      <c r="B63" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E63" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F61" s="9" t="s">
+      <c r="F63" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="72"/>
-      <c r="B62" s="73"/>
-      <c r="C62" s="73"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="74"/>
-      <c r="G62" s="6"/>
-    </row>
-    <row r="63" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="97" t="s">
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="107"/>
+      <c r="B64" s="108"/>
+      <c r="C64" s="108"/>
+      <c r="D64" s="108"/>
+      <c r="E64" s="108"/>
+      <c r="F64" s="109"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F63" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="97"/>
-      <c r="B64" s="7" t="s">
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="103"/>
+      <c r="B66" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7" t="s">
+      <c r="C66" s="7"/>
+      <c r="D66" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F66" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="97"/>
-      <c r="B65" s="7" t="s">
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="103"/>
+      <c r="B67" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7" t="s">
+      <c r="C67" s="7"/>
+      <c r="D67" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F67" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G65" s="6"/>
-    </row>
-    <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="97"/>
-      <c r="B66" s="8" t="s">
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="103"/>
+      <c r="B68" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="8" t="s">
+      <c r="C68" s="7"/>
+      <c r="D68" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F68" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G66" s="6"/>
-    </row>
-    <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="72"/>
-      <c r="B67" s="73"/>
-      <c r="C67" s="73"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="73"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="6"/>
-    </row>
-    <row r="68" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="107"/>
+      <c r="B69" s="108"/>
+      <c r="C69" s="108"/>
+      <c r="D69" s="108"/>
+      <c r="E69" s="108"/>
+      <c r="F69" s="109"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B70" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="17" t="s">
+      <c r="C70" s="14"/>
+      <c r="D70" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E68" s="17" t="s">
+      <c r="E70" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F68" s="18" t="s">
+      <c r="F70" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="75"/>
-      <c r="B69" s="76"/>
-      <c r="C69" s="76"/>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
-      <c r="F69" s="77"/>
-    </row>
-    <row r="70" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="89" t="s">
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="110"/>
+      <c r="B71" s="111"/>
+      <c r="C71" s="111"/>
+      <c r="D71" s="111"/>
+      <c r="E71" s="111"/>
+      <c r="F71" s="112"/>
+    </row>
+    <row r="72" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B72" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="21" t="s">
+      <c r="C72" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="23" t="s">
+      <c r="D72" s="22"/>
+      <c r="E72" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F70" s="22"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="89"/>
-      <c r="B71" s="22" t="s">
+      <c r="F72" s="22"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="95"/>
+      <c r="B73" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22" t="s">
+      <c r="C73" s="22"/>
+      <c r="D73" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="E71" s="24" t="s">
+      <c r="E73" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F71" s="22"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="89"/>
-      <c r="B72" s="22" t="s">
+      <c r="F73" s="22"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="95"/>
+      <c r="B74" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="32" t="s">
+      <c r="C74" s="22"/>
+      <c r="D74" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E72" s="24" t="s">
+      <c r="E74" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="F72" s="22"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="89"/>
-      <c r="B73" s="22" t="s">
+      <c r="F74" s="22"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="95"/>
+      <c r="B75" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="32" t="s">
+      <c r="C75" s="22"/>
+      <c r="D75" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="E73" s="24" t="s">
+      <c r="E75" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="F73" s="22"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="89"/>
-      <c r="B74" s="22" t="s">
+      <c r="F75" s="22"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="95"/>
+      <c r="B76" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="D76" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="E74" s="24" t="s">
+      <c r="E76" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="F74" s="22"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="89"/>
-      <c r="B75" s="22" t="s">
+      <c r="F76" s="22"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="95"/>
+      <c r="B77" s="22" t="s">
         <v>35</v>
-      </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E75" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F75" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="89"/>
-      <c r="B76" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F76" s="22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="89"/>
-      <c r="B77" s="22" t="s">
-        <v>51</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="95"/>
+      <c r="B78" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F78" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="95"/>
+      <c r="B79" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E77" s="24" t="s">
+      <c r="E79" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F77" s="22" t="s">
+      <c r="F79" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="92"/>
-      <c r="B78" s="93"/>
-      <c r="C78" s="93"/>
-      <c r="D78" s="93"/>
-      <c r="E78" s="93"/>
-      <c r="F78" s="94"/>
-    </row>
-    <row r="79" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="25" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="98"/>
+      <c r="B80" s="99"/>
+      <c r="C80" s="99"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="99"/>
+      <c r="F80" s="100"/>
+    </row>
+    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B79" s="27" t="s">
+      <c r="B81" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C79" s="26"/>
-      <c r="D79" s="27" t="s">
+      <c r="C81" s="26"/>
+      <c r="D81" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E79" s="27" t="s">
+      <c r="E81" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="F79" s="28" t="s">
+      <c r="F81" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="55"/>
-      <c r="B80" s="56"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="56"/>
-      <c r="F80" s="57"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="90" t="s">
+    <row r="82" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="116"/>
+      <c r="B82" s="117"/>
+      <c r="C82" s="117"/>
+      <c r="D82" s="117"/>
+      <c r="E82" s="117"/>
+      <c r="F82" s="118"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="B81" s="29" t="s">
+      <c r="B83" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C81" s="29" t="s">
+      <c r="C83" s="29" t="s">
         <v>130</v>
-      </c>
-      <c r="D81" s="29"/>
-      <c r="E81" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="F81" s="29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="90"/>
-      <c r="B82" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>93</v>
-      </c>
-      <c r="F82" s="29"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="90"/>
-      <c r="B83" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C83" s="29" t="s">
-        <v>65</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="30" t="s">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="F83" s="29" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="90"/>
+      <c r="A84" s="96"/>
       <c r="B84" s="29" t="s">
         <v>92</v>
       </c>
       <c r="C84" s="29"/>
-      <c r="D84" s="31" t="s">
+      <c r="D84" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F84" s="29"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="96"/>
+      <c r="B85" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D85" s="29"/>
+      <c r="E85" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="F85" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="96"/>
+      <c r="B86" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="29"/>
+      <c r="D86" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E84" s="30" t="s">
+      <c r="E86" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F84" s="29"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="58"/>
-      <c r="B85" s="59"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="59"/>
-      <c r="E85" s="59"/>
-      <c r="F85" s="60"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="69" t="s">
+      <c r="F86" s="29"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="119"/>
+      <c r="B87" s="120"/>
+      <c r="C87" s="120"/>
+      <c r="D87" s="120"/>
+      <c r="E87" s="120"/>
+      <c r="F87" s="121"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="130" t="s">
         <v>217</v>
       </c>
-      <c r="B86" s="29" t="s">
+      <c r="B88" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C86" s="29" t="s">
+      <c r="C88" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="D86" s="31"/>
-      <c r="E86" s="30" t="s">
+      <c r="D88" s="31"/>
+      <c r="E88" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="F86" s="29"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="70"/>
-      <c r="B87" s="29" t="s">
+      <c r="F88" s="29"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="131"/>
+      <c r="B89" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C87" s="29"/>
-      <c r="D87" s="31" t="s">
+      <c r="C89" s="29"/>
+      <c r="D89" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="E89" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="F87" s="29"/>
-    </row>
-    <row r="88" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="58"/>
-      <c r="B88" s="59"/>
-      <c r="C88" s="59"/>
-      <c r="D88" s="59"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="60"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="91" t="s">
+      <c r="F89" s="29"/>
+    </row>
+    <row r="90" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="119"/>
+      <c r="B90" s="120"/>
+      <c r="C90" s="120"/>
+      <c r="D90" s="120"/>
+      <c r="E90" s="120"/>
+      <c r="F90" s="121"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="97" t="s">
         <v>117</v>
       </c>
-      <c r="B89" s="13" t="s">
+      <c r="B91" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C89" s="13" t="s">
+      <c r="C91" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D89" s="13"/>
-      <c r="E89" s="14" t="s">
+      <c r="D91" s="13"/>
+      <c r="E91" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F89" s="13" t="s">
+      <c r="F91" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="91"/>
-      <c r="B90" s="13" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="97"/>
+      <c r="B92" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13" t="s">
+      <c r="C92" s="13"/>
+      <c r="D92" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E90" s="14" t="s">
+      <c r="E92" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F90" s="13" t="s">
+      <c r="F92" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="58"/>
-      <c r="B91" s="59"/>
-      <c r="C91" s="59"/>
-      <c r="D91" s="59"/>
-      <c r="E91" s="59"/>
-      <c r="F91" s="60"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="88" t="s">
+    <row r="93" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="119"/>
+      <c r="B93" s="120"/>
+      <c r="C93" s="120"/>
+      <c r="D93" s="120"/>
+      <c r="E93" s="120"/>
+      <c r="F93" s="121"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B94" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C94" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D92" s="15"/>
-      <c r="E92" s="16" t="s">
+      <c r="D94" s="15"/>
+      <c r="E94" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F92" s="15" t="s">
+      <c r="F94" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="88"/>
-      <c r="B93" s="15" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="94"/>
+      <c r="B95" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15" t="s">
+      <c r="C95" s="15"/>
+      <c r="D95" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E95" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F93" s="15" t="s">
+      <c r="F95" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="37"/>
-      <c r="E94" s="6"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="78" t="s">
+    <row r="96" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="37"/>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="93" t="s">
         <v>160</v>
       </c>
-      <c r="B95" s="78"/>
-      <c r="C95" s="78"/>
-      <c r="D95" s="78"/>
-      <c r="E95" s="78"/>
-      <c r="F95" s="78"/>
-    </row>
-    <row r="97" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="122"/>
-      <c r="B97" s="123"/>
-      <c r="C97" s="123"/>
-      <c r="D97" s="122"/>
-      <c r="E97" s="122"/>
-    </row>
-    <row r="98" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="124"/>
-      <c r="B98" s="125"/>
-      <c r="C98" s="125"/>
-      <c r="D98" s="126"/>
-      <c r="E98" s="127"/>
-    </row>
-    <row r="99" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="101"/>
-      <c r="B99" s="102"/>
-      <c r="C99" s="102"/>
-      <c r="D99" s="128"/>
-      <c r="E99" s="128"/>
-    </row>
-    <row r="100" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="101"/>
-      <c r="B100" s="102"/>
-      <c r="C100" s="102"/>
-      <c r="D100" s="128"/>
-      <c r="E100" s="128"/>
-    </row>
-    <row r="101" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="101"/>
-      <c r="B101" s="129"/>
-      <c r="C101" s="102"/>
-      <c r="D101" s="128"/>
-      <c r="E101" s="128"/>
-    </row>
-    <row r="102" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="101"/>
-      <c r="B102" s="102"/>
-      <c r="C102" s="102"/>
-      <c r="D102" s="128"/>
-      <c r="E102" s="128"/>
-    </row>
-    <row r="103" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="101"/>
-      <c r="B103" s="102"/>
-      <c r="C103" s="102"/>
-      <c r="D103" s="128"/>
-      <c r="E103" s="128"/>
-    </row>
-    <row r="104" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="101"/>
-      <c r="B104" s="102"/>
-      <c r="C104" s="102"/>
-      <c r="D104" s="128"/>
-      <c r="E104" s="128"/>
-    </row>
-    <row r="105" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="101"/>
-      <c r="B105" s="102"/>
-      <c r="C105" s="102"/>
-      <c r="D105" s="128"/>
-      <c r="E105" s="128"/>
-    </row>
-    <row r="106" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="101"/>
-      <c r="B106" s="102"/>
-      <c r="C106" s="102"/>
-      <c r="D106" s="128"/>
-      <c r="E106" s="128"/>
-    </row>
-    <row r="107" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="101"/>
-      <c r="B107" s="102"/>
-      <c r="C107" s="102"/>
-      <c r="D107" s="128"/>
-      <c r="E107" s="128"/>
-    </row>
-    <row r="108" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="101"/>
-      <c r="B108" s="102"/>
-      <c r="C108" s="102"/>
-      <c r="D108" s="128"/>
-      <c r="E108" s="128"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="130"/>
-      <c r="B109" s="131"/>
-      <c r="C109" s="131"/>
-      <c r="D109" s="128"/>
-      <c r="E109" s="128"/>
-    </row>
-    <row r="110" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="130"/>
-      <c r="B110" s="132"/>
-      <c r="C110" s="132"/>
-      <c r="D110" s="128"/>
-      <c r="E110" s="128"/>
-    </row>
-    <row r="111" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="101"/>
-      <c r="B111" s="102"/>
-      <c r="C111" s="102"/>
-      <c r="D111" s="128"/>
-      <c r="E111" s="128"/>
-    </row>
-    <row r="112" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="101"/>
-      <c r="B112" s="102"/>
-      <c r="C112" s="102"/>
-      <c r="D112" s="128"/>
-      <c r="E112" s="128"/>
-    </row>
-    <row r="113" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="101"/>
-      <c r="B113" s="102"/>
-      <c r="C113" s="102"/>
-      <c r="D113" s="128"/>
-      <c r="E113" s="128"/>
-    </row>
-    <row r="114" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="101"/>
-      <c r="B114" s="102"/>
-      <c r="C114" s="102"/>
-      <c r="D114" s="128"/>
-      <c r="E114" s="128"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="101"/>
-      <c r="B115" s="103"/>
-      <c r="C115" s="103"/>
-      <c r="D115" s="133"/>
-      <c r="E115" s="133"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D116" s="38"/>
-      <c r="E116" s="38"/>
+      <c r="B97" s="93"/>
+      <c r="C97" s="93"/>
+      <c r="D97" s="93"/>
+      <c r="E97" s="93"/>
+      <c r="F97" s="93"/>
+    </row>
+    <row r="99" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="92"/>
+      <c r="B99" s="101"/>
+      <c r="C99" s="101"/>
+      <c r="D99" s="92"/>
+      <c r="E99" s="92"/>
+    </row>
+    <row r="100" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="73"/>
+      <c r="B100" s="74"/>
+      <c r="C100" s="74"/>
+      <c r="D100" s="72"/>
+      <c r="E100" s="75"/>
+    </row>
+    <row r="101" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="B101" s="55"/>
+      <c r="C101" s="55"/>
+      <c r="D101" s="105"/>
+      <c r="E101" s="105"/>
+    </row>
+    <row r="102" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="B102" s="55"/>
+      <c r="C102" s="55"/>
+      <c r="D102" s="105"/>
+      <c r="E102" s="105"/>
+    </row>
+    <row r="103" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="B103" s="76"/>
+      <c r="C103" s="55"/>
+      <c r="D103" s="105"/>
+      <c r="E103" s="105"/>
+    </row>
+    <row r="104" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+      <c r="B104" s="55"/>
+      <c r="C104" s="55"/>
+      <c r="D104" s="105"/>
+      <c r="E104" s="105"/>
+    </row>
+    <row r="105" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+      <c r="B105" s="55"/>
+      <c r="C105" s="55"/>
+      <c r="D105" s="105"/>
+      <c r="E105" s="105"/>
+    </row>
+    <row r="106" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+      <c r="B106" s="55"/>
+      <c r="C106" s="55"/>
+      <c r="D106" s="105"/>
+      <c r="E106" s="105"/>
+    </row>
+    <row r="107" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+      <c r="B107" s="55"/>
+      <c r="C107" s="55"/>
+      <c r="D107" s="105"/>
+      <c r="E107" s="105"/>
+    </row>
+    <row r="108" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2"/>
+      <c r="B108" s="55"/>
+      <c r="C108" s="55"/>
+      <c r="D108" s="105"/>
+      <c r="E108" s="105"/>
+    </row>
+    <row r="109" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2"/>
+      <c r="B109" s="55"/>
+      <c r="C109" s="55"/>
+      <c r="D109" s="105"/>
+      <c r="E109" s="105"/>
+    </row>
+    <row r="110" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+      <c r="B110" s="55"/>
+      <c r="C110" s="55"/>
+      <c r="D110" s="105"/>
+      <c r="E110" s="105"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="104"/>
+      <c r="B111" s="90"/>
+      <c r="C111" s="90"/>
+      <c r="D111" s="105"/>
+      <c r="E111" s="105"/>
+    </row>
+    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="104"/>
+      <c r="B112" s="89"/>
+      <c r="C112" s="89"/>
+      <c r="D112" s="105"/>
+      <c r="E112" s="105"/>
+    </row>
+    <row r="113" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+      <c r="B113" s="55"/>
+      <c r="C113" s="55"/>
+      <c r="D113" s="105"/>
+      <c r="E113" s="105"/>
+    </row>
+    <row r="114" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="2"/>
+      <c r="B114" s="55"/>
+      <c r="C114" s="55"/>
+      <c r="D114" s="105"/>
+      <c r="E114" s="105"/>
+    </row>
+    <row r="115" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="55"/>
+      <c r="C115" s="55"/>
+      <c r="D115" s="105"/>
+      <c r="E115" s="105"/>
+    </row>
+    <row r="116" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2"/>
+      <c r="B116" s="55"/>
+      <c r="C116" s="55"/>
+      <c r="D116" s="105"/>
+      <c r="E116" s="105"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2"/>
+      <c r="B117" s="77"/>
+      <c r="C117" s="77"/>
       <c r="D117" s="38"/>
       <c r="E117" s="38"/>
     </row>
@@ -4040,51 +4043,59 @@
       <c r="D119" s="38"/>
       <c r="E119" s="38"/>
     </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D120" s="38"/>
+      <c r="E120" s="38"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="38"/>
+      <c r="E121" s="38"/>
+    </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="A10:B14"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D18:D33"/>
-    <mergeCell ref="E18:E33"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="A49:F49"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A95:F95"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A70:A77"/>
-    <mergeCell ref="A81:A84"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A51:A61"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="D99:D114"/>
-    <mergeCell ref="E99:E114"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A62:F62"/>
-    <mergeCell ref="A67:F67"/>
+    <mergeCell ref="A64:F64"/>
     <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A71:F71"/>
+    <mergeCell ref="A38:F38"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="A53:A63"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="D101:D116"/>
+    <mergeCell ref="E101:E116"/>
+    <mergeCell ref="A82:F82"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A93:F93"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A72:A79"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A91:A92"/>
     <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A88:F88"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="E40:E45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C40:C45"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="A12:B16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D20:D35"/>
+    <mergeCell ref="E20:E35"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="A97:F97"/>
+    <mergeCell ref="A94:A95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change unregisterd logic add network int flug music play
</commit_message>
<xml_diff>
--- a/doc/CMD list of Face attendence .xlsx
+++ b/doc/CMD list of Face attendence .xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ESP32_lvgl\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FF7388-3D5E-4CB7-9965-1A1EC9FA2164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1C0390-F75E-40F6-8CA7-530FBEDB9029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="15720" tabRatio="537" xr2:uid="{954E009C-196F-4536-BE3A-69B99BC5250B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$52:$F$83</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$56:$F$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="246">
   <si>
     <t>ping</t>
   </si>
@@ -1567,6 +1567,21 @@
   </si>
   <si>
     <t>0xFFFF</t>
+  </si>
+  <si>
+    <t>Music no</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>Unregistered</t>
+  </si>
+  <si>
+    <t>Welcome to our THT company</t>
+  </si>
+  <si>
+    <t>Voice</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +1994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2149,6 +2164,126 @@
     <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2191,127 +2326,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2657,10 +2681,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:N125"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,28 +2706,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="77" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="106"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
     </row>
     <row r="4" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="114"/>
+      <c r="B4" s="86"/>
     </row>
     <row r="5" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
@@ -2738,1364 +2762,1396 @@
       </c>
     </row>
     <row r="9" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="113" t="s">
+    <row r="10" spans="1:6" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="134" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="134" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="132">
+        <v>1</v>
+      </c>
+      <c r="B11" s="133" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="132">
+        <v>2</v>
+      </c>
+      <c r="B12" s="133" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="132">
+        <v>3</v>
+      </c>
+      <c r="B13" s="133" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" s="42" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="85" t="s">
         <v>227</v>
       </c>
-      <c r="B11" s="114"/>
-      <c r="C11" s="56" t="s">
+      <c r="B15" s="86"/>
+      <c r="C15" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D15" s="56" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="67"/>
-    </row>
-    <row r="12" spans="1:6" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
+      <c r="E15" s="67"/>
+    </row>
+    <row r="16" spans="1:6" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="62" t="s">
+      <c r="B16" s="118"/>
+      <c r="C16" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="D12" s="57" t="s">
+      <c r="D16" s="57" t="s">
         <v>226</v>
       </c>
-      <c r="E12" s="68"/>
-    </row>
-    <row r="13" spans="1:6" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="78"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="61" t="s">
+      <c r="E16" s="68"/>
+    </row>
+    <row r="17" spans="1:5" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="118"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="61" t="s">
         <v>234</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D17" s="58" t="s">
         <v>224</v>
       </c>
-      <c r="E13" s="68"/>
-    </row>
-    <row r="14" spans="1:6" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="63" t="s">
+      <c r="E17" s="68"/>
+    </row>
+    <row r="18" spans="1:5" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="118"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D18" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="E14" s="68"/>
-    </row>
-    <row r="15" spans="1:6" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="65" t="s">
+      <c r="E18" s="68"/>
+    </row>
+    <row r="19" spans="1:5" s="42" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="118"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="65" t="s">
         <v>236</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D19" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="E15" s="68"/>
-    </row>
-    <row r="16" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="66" t="s">
+      <c r="E19" s="68"/>
+    </row>
+    <row r="20" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="118"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="66" t="s">
         <v>237</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D20" s="60" t="s">
         <v>225</v>
       </c>
-      <c r="E16" s="68"/>
-    </row>
-    <row r="17" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
-      <c r="B17" s="70"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="68"/>
-    </row>
-    <row r="18" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="79" t="s">
+      <c r="E20" s="68"/>
+    </row>
+    <row r="21" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="70"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="68"/>
+    </row>
+    <row r="22" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="119" t="s">
         <v>162</v>
       </c>
-      <c r="B18" s="80"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="79" t="s">
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="119" t="s">
         <v>179</v>
       </c>
-      <c r="E18" s="79"/>
-    </row>
-    <row r="19" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="47" t="s">
+      <c r="E22" s="119"/>
+    </row>
+    <row r="23" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B23" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C23" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D23" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E23" s="41" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="81" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" s="81" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-    </row>
-    <row r="22" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="5">
-        <v>45575.507002314815</v>
-      </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-    </row>
-    <row r="23" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
     </row>
     <row r="24" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
+        <v>151</v>
+      </c>
+      <c r="D24" s="121" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" s="121" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="25" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
       <c r="C25" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
+        <v>126</v>
+      </c>
+      <c r="D25" s="121"/>
+      <c r="E25" s="121"/>
     </row>
     <row r="26" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="4">
-        <v>11000</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
+        <v>72</v>
+      </c>
+      <c r="B26" s="5">
+        <v>45575.507002314815</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
     </row>
     <row r="27" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="4">
-        <v>100</v>
+        <v>73</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
+        <v>152</v>
+      </c>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
     </row>
     <row r="28" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="4">
-        <v>110</v>
+        <v>75</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
+        <v>79</v>
+      </c>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
     </row>
     <row r="29" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="4">
-        <v>11</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B29" s="4"/>
       <c r="C29" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
+        <v>77</v>
+      </c>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
     </row>
     <row r="30" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" s="84" t="s">
-        <v>210</v>
-      </c>
-      <c r="C30" s="85"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="81"/>
+      <c r="A30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="4">
+        <v>11000</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
     </row>
     <row r="31" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="86" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" s="87"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="81"/>
+      <c r="A31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="4">
+        <v>100</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
     </row>
     <row r="32" spans="1:5" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>144</v>
+        <v>84</v>
+      </c>
+      <c r="B32" s="4">
+        <v>110</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
+        <v>87</v>
+      </c>
+      <c r="D32" s="121"/>
+      <c r="E32" s="121"/>
     </row>
     <row r="33" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>146</v>
+        <v>85</v>
+      </c>
+      <c r="B33" s="4">
+        <v>11</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
+        <v>88</v>
+      </c>
+      <c r="D33" s="121"/>
+      <c r="E33" s="121"/>
     </row>
     <row r="34" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="4">
-        <v>6</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
+      <c r="A34" s="122" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="124" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="125"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
     </row>
     <row r="35" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B35" s="4">
-        <v>10</v>
-      </c>
-      <c r="C35" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="126" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="127"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="121"/>
     </row>
     <row r="36" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+    </row>
+    <row r="37" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="121"/>
+      <c r="E37" s="121"/>
+    </row>
+    <row r="38" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="4">
+        <v>6</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="121"/>
+      <c r="E38" s="121"/>
+    </row>
+    <row r="39" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="4">
+        <v>10</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="121"/>
+      <c r="E39" s="121"/>
+    </row>
+    <row r="40" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B36" s="88" t="s">
+      <c r="B40" s="128" t="s">
         <v>229</v>
       </c>
-      <c r="C36" s="88"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-    </row>
-    <row r="37" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="69"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="68"/>
-    </row>
-    <row r="38" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="93" t="s">
+      <c r="C40" s="128"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+    </row>
+    <row r="41" spans="1:6" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="70"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="68"/>
+    </row>
+    <row r="42" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="84" t="s">
         <v>161</v>
       </c>
-      <c r="B38" s="93"/>
-      <c r="C38" s="93"/>
-      <c r="D38" s="93"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="93"/>
-    </row>
-    <row r="39" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="115" t="s">
+      <c r="B42" s="84"/>
+      <c r="C42" s="84"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="84"/>
+      <c r="F42" s="84"/>
+    </row>
+    <row r="43" spans="1:6" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="87" t="s">
         <v>191</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-    </row>
-    <row r="41" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51" t="s">
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="88"/>
+    </row>
+    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B45" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C45" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D45" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="E45" s="33" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="C42" s="127"/>
-      <c r="D42" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="E42" s="124" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="C43" s="129"/>
-      <c r="D43" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E43" s="125"/>
-    </row>
-    <row r="44" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="C44" s="129"/>
-      <c r="D44" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="E44" s="125"/>
-    </row>
-    <row r="45" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="C45" s="129"/>
-      <c r="D45" s="36" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="125"/>
     </row>
     <row r="46" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="94"/>
+      <c r="D46" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="91" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C47" s="96"/>
+      <c r="D47" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E47" s="92"/>
+    </row>
+    <row r="48" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" s="96"/>
+      <c r="D48" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="E48" s="92"/>
+    </row>
+    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="96"/>
+      <c r="D49" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="92"/>
+    </row>
+    <row r="50" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B50" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C46" s="129"/>
-      <c r="D46" s="36" t="s">
+      <c r="C50" s="96"/>
+      <c r="D50" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="E46" s="125"/>
-    </row>
-    <row r="47" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="52" t="s">
+      <c r="E50" s="92"/>
+    </row>
+    <row r="51" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="52" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B51" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="C47" s="128"/>
-      <c r="D47" s="36" t="s">
+      <c r="C51" s="95"/>
+      <c r="D51" s="36" t="s">
         <v>209</v>
       </c>
-      <c r="E47" s="126"/>
-    </row>
-    <row r="48" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="s">
+      <c r="E51" s="93"/>
+    </row>
+    <row r="52" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B48" s="127"/>
-      <c r="C48" s="53" t="s">
+      <c r="B52" s="94"/>
+      <c r="C52" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="50" t="s">
+      <c r="D52" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="E48" s="122" t="s">
+      <c r="E52" s="89" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="43" t="s">
+    <row r="53" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B49" s="128"/>
-      <c r="C49" s="54" t="s">
+      <c r="B53" s="95"/>
+      <c r="C53" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="D49" s="44" t="s">
+      <c r="D53" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="E49" s="123"/>
-    </row>
-    <row r="51" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="91" t="s">
+      <c r="E53" s="90"/>
+    </row>
+    <row r="55" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="B51" s="91"/>
-      <c r="C51" s="91"/>
-      <c r="D51" s="91"/>
-      <c r="E51" s="91"/>
-      <c r="F51" s="91"/>
-    </row>
-    <row r="52" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A52" s="46" t="s">
+      <c r="B55" s="88"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="88"/>
+      <c r="F55" s="88"/>
+    </row>
+    <row r="56" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A56" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="46" t="s">
+      <c r="B56" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="46" t="s">
+      <c r="C56" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="46" t="s">
+      <c r="D56" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E52" s="46" t="s">
+      <c r="E56" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="F52" s="46" t="s">
+      <c r="F56" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="G52" s="6"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="102" t="s">
+      <c r="G56" s="6"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="97" t="s">
         <v>128</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B57" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10" t="s">
+      <c r="D57" s="10"/>
+      <c r="E57" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F57" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G53" s="6"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="102"/>
-      <c r="B54" s="9" t="s">
+      <c r="G57" s="6"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="97"/>
+      <c r="B58" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E58" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F58" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G54" s="6"/>
-    </row>
-    <row r="55" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="102"/>
-      <c r="B55" s="9" t="s">
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="97"/>
+      <c r="B59" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="9"/>
-      <c r="E55" s="10" t="s">
+      <c r="D59" s="9"/>
+      <c r="E59" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="6"/>
-    </row>
-    <row r="56" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="102"/>
-      <c r="B56" s="10" t="s">
+      <c r="F59" s="12"/>
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="97"/>
+      <c r="B60" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="11" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E60" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F60" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G56" s="6"/>
-    </row>
-    <row r="57" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="102"/>
-      <c r="B57" s="10" t="s">
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="97"/>
+      <c r="B61" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="11" t="s">
+      <c r="C61" s="9"/>
+      <c r="D61" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E61" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F61" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="G57" s="6"/>
-    </row>
-    <row r="58" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="102"/>
-      <c r="B58" s="9" t="s">
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="97"/>
+      <c r="B62" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C62" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9" t="s">
+      <c r="D62" s="9"/>
+      <c r="E62" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="6"/>
-    </row>
-    <row r="59" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="102"/>
-      <c r="B59" s="9" t="s">
+      <c r="F62" s="9"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="97"/>
+      <c r="B63" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="F59" s="9"/>
-      <c r="G59" s="6"/>
-    </row>
-    <row r="60" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="102"/>
-      <c r="B60" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F60" s="9"/>
-      <c r="G60" s="6"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="102"/>
-      <c r="B61" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="102"/>
-      <c r="B62" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G62" s="6"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="102"/>
-      <c r="B63" s="9" t="s">
-        <v>8</v>
       </c>
       <c r="C63" s="9"/>
       <c r="D63" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63" s="9"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="97"/>
+      <c r="B64" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="97"/>
+      <c r="B65" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="97"/>
+      <c r="B66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="97"/>
+      <c r="B67" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E67" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F63" s="9" t="s">
+      <c r="F67" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="107"/>
-      <c r="B64" s="108"/>
-      <c r="C64" s="108"/>
-      <c r="D64" s="108"/>
-      <c r="E64" s="108"/>
-      <c r="F64" s="109"/>
-      <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="103" t="s">
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="78"/>
+      <c r="B68" s="79"/>
+      <c r="C68" s="79"/>
+      <c r="D68" s="79"/>
+      <c r="E68" s="79"/>
+      <c r="F68" s="80"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D69" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F69" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G65" s="6"/>
-    </row>
-    <row r="66" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="103"/>
-      <c r="B66" s="7" t="s">
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="98"/>
+      <c r="B70" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7" t="s">
+      <c r="C70" s="7"/>
+      <c r="D70" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G66" s="6"/>
-    </row>
-    <row r="67" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="103"/>
-      <c r="B67" s="7" t="s">
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="98"/>
+      <c r="B71" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7" t="s">
+      <c r="C71" s="7"/>
+      <c r="D71" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G67" s="6"/>
-    </row>
-    <row r="68" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="103"/>
-      <c r="B68" s="8" t="s">
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="98"/>
+      <c r="B72" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="8" t="s">
+      <c r="C72" s="7"/>
+      <c r="D72" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F72" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="107"/>
-      <c r="B69" s="108"/>
-      <c r="C69" s="108"/>
-      <c r="D69" s="108"/>
-      <c r="E69" s="108"/>
-      <c r="F69" s="109"/>
-      <c r="G69" s="6"/>
-    </row>
-    <row r="70" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="78"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="79"/>
+      <c r="D73" s="79"/>
+      <c r="E73" s="79"/>
+      <c r="F73" s="80"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="1:7" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A74" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B74" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="17" t="s">
+      <c r="C74" s="14"/>
+      <c r="D74" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E74" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="F70" s="18" t="s">
+      <c r="F74" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="G70" s="6"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="110"/>
-      <c r="B71" s="111"/>
-      <c r="C71" s="111"/>
-      <c r="D71" s="111"/>
-      <c r="E71" s="111"/>
-      <c r="F71" s="112"/>
-    </row>
-    <row r="72" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="95" t="s">
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="81"/>
+      <c r="B75" s="82"/>
+      <c r="C75" s="82"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="82"/>
+      <c r="F75" s="83"/>
+    </row>
+    <row r="76" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="109" t="s">
         <v>32</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B76" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C76" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D72" s="22"/>
-      <c r="E72" s="23" t="s">
+      <c r="D76" s="22"/>
+      <c r="E76" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F72" s="22"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="95"/>
-      <c r="B73" s="22" t="s">
+      <c r="F76" s="22"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="109"/>
+      <c r="B77" s="22" t="s">
         <v>36</v>
-      </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E73" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="F73" s="22"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="95"/>
-      <c r="B74" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="E74" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F74" s="22"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="95"/>
-      <c r="B75" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E75" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F75" s="22"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="95"/>
-      <c r="B76" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="F76" s="22"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="95"/>
-      <c r="B77" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F77" s="22"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="109"/>
+      <c r="B78" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78" s="22"/>
+      <c r="D78" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F78" s="22"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="109"/>
+      <c r="B79" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E79" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="F79" s="22"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="109"/>
+      <c r="B80" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F80" s="22"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="109"/>
+      <c r="B81" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E77" s="24" t="s">
+      <c r="E81" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="F77" s="22" t="s">
+      <c r="F81" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="95"/>
-      <c r="B78" s="22" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="109"/>
+      <c r="B82" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22" t="s">
+      <c r="C82" s="22"/>
+      <c r="D82" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E78" s="24" t="s">
+      <c r="E82" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F78" s="22" t="s">
+      <c r="F82" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="95"/>
-      <c r="B79" s="22" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="109"/>
+      <c r="B83" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="22" t="s">
+      <c r="C83" s="22"/>
+      <c r="D83" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E83" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F79" s="22" t="s">
+      <c r="F83" s="22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="98"/>
-      <c r="B80" s="99"/>
-      <c r="C80" s="99"/>
-      <c r="D80" s="99"/>
-      <c r="E80" s="99"/>
-      <c r="F80" s="100"/>
-    </row>
-    <row r="81" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="25" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="112"/>
+      <c r="B84" s="113"/>
+      <c r="C84" s="113"/>
+      <c r="D84" s="113"/>
+      <c r="E84" s="113"/>
+      <c r="F84" s="114"/>
+    </row>
+    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="27" t="s">
+      <c r="B85" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C81" s="26"/>
-      <c r="D81" s="27" t="s">
+      <c r="C85" s="26"/>
+      <c r="D85" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E81" s="27" t="s">
+      <c r="E85" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="F81" s="28" t="s">
+      <c r="F85" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="116"/>
-      <c r="B82" s="117"/>
-      <c r="C82" s="117"/>
-      <c r="D82" s="117"/>
-      <c r="E82" s="117"/>
-      <c r="F82" s="118"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="96" t="s">
+    <row r="86" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="101"/>
+      <c r="B86" s="102"/>
+      <c r="C86" s="102"/>
+      <c r="D86" s="102"/>
+      <c r="E86" s="102"/>
+      <c r="F86" s="103"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="29" t="s">
+      <c r="B87" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C83" s="29" t="s">
+      <c r="C87" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="D83" s="29"/>
-      <c r="E83" s="30" t="s">
+      <c r="D87" s="29"/>
+      <c r="E87" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="F83" s="29" t="s">
+      <c r="F87" s="29" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="96"/>
-      <c r="B84" s="29" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="110"/>
+      <c r="B88" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29" t="s">
+      <c r="C88" s="29"/>
+      <c r="D88" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E84" s="30" t="s">
+      <c r="E88" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F84" s="29"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="96"/>
-      <c r="B85" s="29" t="s">
+      <c r="F88" s="29"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="110"/>
+      <c r="B89" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="29" t="s">
+      <c r="C89" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="D85" s="29"/>
-      <c r="E85" s="30" t="s">
+      <c r="D89" s="29"/>
+      <c r="E89" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F85" s="29" t="s">
+      <c r="F89" s="29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="96"/>
-      <c r="B86" s="29" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="110"/>
+      <c r="B90" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C86" s="29"/>
-      <c r="D86" s="31" t="s">
+      <c r="C90" s="29"/>
+      <c r="D90" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E86" s="30" t="s">
+      <c r="E90" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F86" s="29"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="119"/>
-      <c r="B87" s="120"/>
-      <c r="C87" s="120"/>
-      <c r="D87" s="120"/>
-      <c r="E87" s="120"/>
-      <c r="F87" s="121"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="130" t="s">
+      <c r="F90" s="29"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="104"/>
+      <c r="B91" s="105"/>
+      <c r="C91" s="105"/>
+      <c r="D91" s="105"/>
+      <c r="E91" s="105"/>
+      <c r="F91" s="106"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="B88" s="29" t="s">
+      <c r="B92" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="C88" s="29" t="s">
+      <c r="C92" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="D88" s="31"/>
-      <c r="E88" s="30" t="s">
+      <c r="D92" s="31"/>
+      <c r="E92" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="F88" s="29"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="131"/>
-      <c r="B89" s="29" t="s">
+      <c r="F92" s="29"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="108"/>
+      <c r="B93" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C89" s="29"/>
-      <c r="D89" s="31" t="s">
+      <c r="C93" s="29"/>
+      <c r="D93" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="E89" s="30" t="s">
+      <c r="E93" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="F89" s="29"/>
-    </row>
-    <row r="90" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="119"/>
-      <c r="B90" s="120"/>
-      <c r="C90" s="120"/>
-      <c r="D90" s="120"/>
-      <c r="E90" s="120"/>
-      <c r="F90" s="121"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="97" t="s">
+      <c r="F93" s="29"/>
+    </row>
+    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="104"/>
+      <c r="B94" s="105"/>
+      <c r="C94" s="105"/>
+      <c r="D94" s="105"/>
+      <c r="E94" s="105"/>
+      <c r="F94" s="106"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="111" t="s">
         <v>117</v>
       </c>
-      <c r="B91" s="13" t="s">
+      <c r="B95" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C95" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D91" s="13"/>
-      <c r="E91" s="14" t="s">
+      <c r="D95" s="13"/>
+      <c r="E95" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F91" s="13" t="s">
+      <c r="F95" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="97"/>
-      <c r="B92" s="13" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="111"/>
+      <c r="B96" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13" t="s">
+      <c r="C96" s="13"/>
+      <c r="D96" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E92" s="14" t="s">
+      <c r="E96" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F92" s="13" t="s">
+      <c r="F96" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="119"/>
-      <c r="B93" s="120"/>
-      <c r="C93" s="120"/>
-      <c r="D93" s="120"/>
-      <c r="E93" s="120"/>
-      <c r="F93" s="121"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="94" t="s">
+    <row r="97" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="104"/>
+      <c r="B97" s="105"/>
+      <c r="C97" s="105"/>
+      <c r="D97" s="105"/>
+      <c r="E97" s="105"/>
+      <c r="F97" s="106"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="131" t="s">
         <v>43</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B98" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C98" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D94" s="15"/>
-      <c r="E94" s="16" t="s">
+      <c r="D98" s="15"/>
+      <c r="E98" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F94" s="15" t="s">
+      <c r="F98" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="94"/>
-      <c r="B95" s="15" t="s">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="131"/>
+      <c r="B99" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C95" s="15"/>
-      <c r="D95" s="15" t="s">
+      <c r="C99" s="15"/>
+      <c r="D99" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E99" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F95" s="15" t="s">
+      <c r="F99" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="37"/>
-      <c r="E96" s="6"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="93" t="s">
+    <row r="100" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="37"/>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="84" t="s">
         <v>160</v>
       </c>
-      <c r="B97" s="93"/>
-      <c r="C97" s="93"/>
-      <c r="D97" s="93"/>
-      <c r="E97" s="93"/>
-      <c r="F97" s="93"/>
-    </row>
-    <row r="99" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="92"/>
-      <c r="B99" s="101"/>
-      <c r="C99" s="101"/>
-      <c r="D99" s="92"/>
-      <c r="E99" s="92"/>
-    </row>
-    <row r="100" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="73"/>
-      <c r="B100" s="74"/>
-      <c r="C100" s="74"/>
-      <c r="D100" s="72"/>
-      <c r="E100" s="75"/>
-    </row>
-    <row r="101" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
-      <c r="B101" s="55"/>
-      <c r="C101" s="55"/>
-      <c r="D101" s="105"/>
-      <c r="E101" s="105"/>
-    </row>
-    <row r="102" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
-      <c r="B102" s="55"/>
-      <c r="C102" s="55"/>
-      <c r="D102" s="105"/>
-      <c r="E102" s="105"/>
-    </row>
-    <row r="103" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-      <c r="B103" s="76"/>
-      <c r="C103" s="55"/>
-      <c r="D103" s="105"/>
-      <c r="E103" s="105"/>
-    </row>
-    <row r="104" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
-      <c r="B104" s="55"/>
-      <c r="C104" s="55"/>
-      <c r="D104" s="105"/>
-      <c r="E104" s="105"/>
-    </row>
-    <row r="105" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="84"/>
+      <c r="C101" s="84"/>
+      <c r="D101" s="84"/>
+      <c r="E101" s="84"/>
+      <c r="F101" s="84"/>
+    </row>
+    <row r="103" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="115"/>
+      <c r="B103" s="116"/>
+      <c r="C103" s="116"/>
+      <c r="D103" s="115"/>
+      <c r="E103" s="115"/>
+    </row>
+    <row r="104" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="73"/>
+      <c r="B104" s="74"/>
+      <c r="C104" s="74"/>
+      <c r="D104" s="72"/>
+      <c r="E104" s="75"/>
+    </row>
+    <row r="105" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="55"/>
       <c r="C105" s="55"/>
-      <c r="D105" s="105"/>
-      <c r="E105" s="105"/>
-    </row>
-    <row r="106" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="100"/>
+      <c r="E105" s="100"/>
+    </row>
+    <row r="106" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="55"/>
       <c r="C106" s="55"/>
-      <c r="D106" s="105"/>
-      <c r="E106" s="105"/>
-    </row>
-    <row r="107" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="100"/>
+      <c r="E106" s="100"/>
+    </row>
+    <row r="107" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
-      <c r="B107" s="55"/>
+      <c r="B107" s="76"/>
       <c r="C107" s="55"/>
-      <c r="D107" s="105"/>
-      <c r="E107" s="105"/>
-    </row>
-    <row r="108" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="100"/>
+      <c r="E107" s="100"/>
+    </row>
+    <row r="108" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="55"/>
       <c r="C108" s="55"/>
-      <c r="D108" s="105"/>
-      <c r="E108" s="105"/>
-    </row>
-    <row r="109" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D108" s="100"/>
+      <c r="E108" s="100"/>
+    </row>
+    <row r="109" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="55"/>
       <c r="C109" s="55"/>
-      <c r="D109" s="105"/>
-      <c r="E109" s="105"/>
+      <c r="D109" s="100"/>
+      <c r="E109" s="100"/>
     </row>
     <row r="110" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="55"/>
       <c r="C110" s="55"/>
-      <c r="D110" s="105"/>
-      <c r="E110" s="105"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="104"/>
-      <c r="B111" s="90"/>
-      <c r="C111" s="90"/>
-      <c r="D111" s="105"/>
-      <c r="E111" s="105"/>
-    </row>
-    <row r="112" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="104"/>
-      <c r="B112" s="89"/>
-      <c r="C112" s="89"/>
-      <c r="D112" s="105"/>
-      <c r="E112" s="105"/>
-    </row>
-    <row r="113" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="100"/>
+      <c r="E110" s="100"/>
+    </row>
+    <row r="111" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="2"/>
+      <c r="B111" s="55"/>
+      <c r="C111" s="55"/>
+      <c r="D111" s="100"/>
+      <c r="E111" s="100"/>
+    </row>
+    <row r="112" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2"/>
+      <c r="B112" s="55"/>
+      <c r="C112" s="55"/>
+      <c r="D112" s="100"/>
+      <c r="E112" s="100"/>
+    </row>
+    <row r="113" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="55"/>
       <c r="C113" s="55"/>
-      <c r="D113" s="105"/>
-      <c r="E113" s="105"/>
-    </row>
-    <row r="114" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="100"/>
+      <c r="E113" s="100"/>
+    </row>
+    <row r="114" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="55"/>
       <c r="C114" s="55"/>
-      <c r="D114" s="105"/>
-      <c r="E114" s="105"/>
-    </row>
-    <row r="115" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2"/>
-      <c r="B115" s="55"/>
-      <c r="C115" s="55"/>
-      <c r="D115" s="105"/>
-      <c r="E115" s="105"/>
-    </row>
-    <row r="116" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2"/>
-      <c r="B116" s="55"/>
-      <c r="C116" s="55"/>
-      <c r="D116" s="105"/>
-      <c r="E116" s="105"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D114" s="100"/>
+      <c r="E114" s="100"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="99"/>
+      <c r="B115" s="130"/>
+      <c r="C115" s="130"/>
+      <c r="D115" s="100"/>
+      <c r="E115" s="100"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="99"/>
+      <c r="B116" s="129"/>
+      <c r="C116" s="129"/>
+      <c r="D116" s="100"/>
+      <c r="E116" s="100"/>
+    </row>
+    <row r="117" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
-      <c r="B117" s="77"/>
-      <c r="C117" s="77"/>
-      <c r="D117" s="38"/>
-      <c r="E117" s="38"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D118" s="38"/>
-      <c r="E118" s="38"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D119" s="38"/>
-      <c r="E119" s="38"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D120" s="38"/>
-      <c r="E120" s="38"/>
+      <c r="B117" s="55"/>
+      <c r="C117" s="55"/>
+      <c r="D117" s="100"/>
+      <c r="E117" s="100"/>
+    </row>
+    <row r="118" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2"/>
+      <c r="B118" s="55"/>
+      <c r="C118" s="55"/>
+      <c r="D118" s="100"/>
+      <c r="E118" s="100"/>
+    </row>
+    <row r="119" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2"/>
+      <c r="B119" s="55"/>
+      <c r="C119" s="55"/>
+      <c r="D119" s="100"/>
+      <c r="E119" s="100"/>
+    </row>
+    <row r="120" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2"/>
+      <c r="B120" s="55"/>
+      <c r="C120" s="55"/>
+      <c r="D120" s="100"/>
+      <c r="E120" s="100"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="2"/>
+      <c r="B121" s="117"/>
+      <c r="C121" s="117"/>
       <c r="D121" s="38"/>
       <c r="E121" s="38"/>
     </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D122" s="38"/>
+      <c r="E122" s="38"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D123" s="38"/>
+      <c r="E123" s="38"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D124" s="38"/>
+      <c r="E124" s="38"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D125" s="38"/>
+      <c r="E125" s="38"/>
+    </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="A16:B20"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:D39"/>
+    <mergeCell ref="E24:E39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="A55:F55"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="A101:F101"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A76:A83"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A103:C103"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="D105:D120"/>
+    <mergeCell ref="E105:E120"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A94:F94"/>
+    <mergeCell ref="A97:F97"/>
+    <mergeCell ref="A91:F91"/>
+    <mergeCell ref="A92:A93"/>
     <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A64:F64"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A71:F71"/>
-    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="A68:F68"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A42:F42"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="E42:E47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="A53:A63"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="D101:D116"/>
-    <mergeCell ref="E101:E116"/>
-    <mergeCell ref="A82:F82"/>
-    <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A93:F93"/>
-    <mergeCell ref="A87:F87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A72:A79"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="A12:B16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D20:D35"/>
-    <mergeCell ref="E20:E35"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="A97:F97"/>
-    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="E46:E51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C46:C51"/>
+    <mergeCell ref="A57:A67"/>
+    <mergeCell ref="A69:A72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>